<commit_message>
method name same as sheet name in excel sheet
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -27,7 +27,7 @@
     <sheet name="removeUsersFromRole" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="getUserActions" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="getRolesAuthenticatedUser" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="getGetAccounts" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="getAccounts" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -869,19 +869,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -2412,9 +2412,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2475,9 +2475,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="42.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2540,7 +2540,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2579,7 +2579,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2619,7 +2619,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2735,7 +2735,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="25" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2774,9 +2774,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2837,9 +2837,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="79.9109311740891"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="80.5546558704453"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2889,10 +2889,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="55.914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="67.7004048582996"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.5991902834008"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="68.2348178137652"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="58.5951417004049"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,14 +2951,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="53.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3011,9 +3011,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="44.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="46.3805668016194"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3063,9 +3063,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="100.797570850202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="47.8825910931174"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="101.655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="45.417004048583"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="19" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="19" width="9.10526315789474"/>
   </cols>
@@ -3116,9 +3116,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="59.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="59.7732793522267"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="19" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="19" width="9.10526315789474"/>
   </cols>
@@ -3169,9 +3169,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="56.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="56.663967611336"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3221,9 +3221,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="53.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="54.2024291497976"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3273,9 +3273,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="49.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="49.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -3325,9 +3325,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="45.0971659919028"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
corporate-account dont until add account affiliation
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="API Request Matrix" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,6 +28,11 @@
     <sheet name="getUserActions" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="getRolesAuthenticatedUser" sheetId="19" state="visible" r:id="rId20"/>
     <sheet name="getAccounts" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="insertAccounts" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="updateAccounts" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="deleteAccounts" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="getAccountContacts" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="addAccountContactAffiliations" sheetId="25" state="visible" r:id="rId26"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="136">
   <si>
     <t>Api</t>
   </si>
@@ -453,6 +458,48 @@
   </si>
   <si>
     <t>jsonSchema/corporate/account/getAccounts.json</t>
+  </si>
+  <si>
+    <t>http://10.0.0.111:8080/web-corporate/api/submit/corporate/account/insertAccounts</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/insertAccounts.json</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/updateAccounts</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"Accounts":[{"AccountID":38,"oca":1}]}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/updateAccounts.json</t>
+  </si>
+  <si>
+    <t>http://10.0.0.111:8080/web-corporate/api/submit/corporate/account/deleteAccounts</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"AccountIDs": [43}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/deleteAccounts.json</t>
+  </si>
+  <si>
+    <t>http://10.0.0.111:8080/web-corporate/api/submit/corporate/account/getAccountContacts</t>
+  </si>
+  <si>
+    <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"DESC"}]},"Params":{"AcountIDs":[40]}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getAccountContacts.json</t>
+  </si>
+  <si>
+    <t>http://10.0.0.111:8080/web-corporate/api/submit/corporate/account/addAccountContactAffiliations</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"AccountIDs":[39,40],"ContactIDs":[1,2],"AffiliationTypeIDs":[1,2]}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/addAccountContactAffiliations.json</t>
   </si>
 </sst>
 </file>
@@ -861,27 +908,27 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topRight" activeCell="F30" activeCellId="1" sqref="C:C F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -2406,15 +2453,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="47.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2469,15 +2516,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="46.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2532,15 +2579,15 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C:C A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2573,13 +2620,13 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C:C B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2612,8 +2659,8 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C:C A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2652,8 +2699,8 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C:C A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2690,8 +2737,8 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C:C A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2728,14 +2775,14 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C:C A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="25" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2768,15 +2815,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="C:C B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.2348178137652"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2831,15 +2878,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="1" sqref="C:C B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="80.5546558704453"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="87.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="50.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2883,16 +2930,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C:C A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="56.3441295546559"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="68.2348178137652"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="43.919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="61.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="63.7368421052632"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2950,15 +2997,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="53.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="82.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="50.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2988,6 +3035,272 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://10.0.0.111:8080/web-corporate/api/submit/corporate/account/getAccounts"/>
   </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C:C"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="66.6275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="25" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C:C"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="66.6275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://localhost:8080/web-corporate/api/submit/corporate/account/updateAccounts"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C:C"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="66.6275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="C:C A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://10.0.0.111:8080/web-corporate/api/submit/corporate/account/getAccountContacts"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="77.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="91.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="53.7246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="25" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3005,15 +3318,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C:C B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="45.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="50.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3057,15 +3370,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C:C B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="101.655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="111.080971659919"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="49.2753036437247"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="19" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="19" width="9.10526315789474"/>
   </cols>
@@ -3110,15 +3423,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C:C A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="59.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="65.1295546558705"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="19" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="19" width="9.10526315789474"/>
   </cols>
@@ -3163,15 +3476,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="56.663967611336"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="35.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="61.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3215,15 +3528,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="54.2024291497976"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3267,15 +3580,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="54.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -3319,15 +3632,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="49.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="19" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
corporate user insert done update added
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,6 +36,8 @@
     <sheet name="deleteAccounts" sheetId="26" state="visible" r:id="rId27"/>
     <sheet name="getAccountContacts" sheetId="27" state="visible" r:id="rId28"/>
     <sheet name="addAccountContactAffiliations" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="insertUser" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="updateUser" sheetId="30" state="visible" r:id="rId31"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="147">
   <si>
     <t>URL</t>
   </si>
@@ -512,6 +514,18 @@
   </si>
   <si>
     <t>jsonSchema/corporate/account/addAccountContactAffiliations.json</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/web-corporate/api/submit/corporate/user/insertUser</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/user/insertUser.json</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/web-corporate/api/submit/corporate/user/updateUser</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/user/updateUser.json</t>
   </si>
 </sst>
 </file>
@@ -523,7 +537,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -597,6 +611,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -718,7 +738,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -839,6 +859,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -920,16 +944,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.7935222672065"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.2550607287449"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.8056680161943"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="66.412955465587"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,15 +997,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.4858299595142"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1025,15 +1049,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.1295546558704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.5587044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1077,15 +1101,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.0971659919028"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1129,15 +1153,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1192,15 +1216,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.7408906882591"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1255,7 +1279,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1296,7 +1320,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1335,7 +1359,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1375,7 +1399,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1413,7 +1437,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1451,16 +1475,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.9676113360324"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="66.8866396761134"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="66.412955465587"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,14 +1528,14 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1544,15 +1568,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.3400809716599"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1607,15 +1631,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1659,15 +1683,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="94.1578947368421"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1711,15 +1735,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="71.2348178137652"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1763,15 +1787,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="48.8461538461539"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1815,15 +1839,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="72.6275303643725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.2712550607288"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="48.8461538461539"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1867,15 +1891,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.3036437246964"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1919,15 +1943,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="94.6923076923077"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="95.5506072874494"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1951,6 +1975,58 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.3562753036437"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1971,15 +2047,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2003,6 +2079,58 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.3562753036437"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2151,7 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F30" activeCellId="0" sqref="F30"/>
@@ -2031,19 +2159,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -3568,16 +3696,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.165991902834"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="66.412955465587"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,15 +3759,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3805668016194"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3686,15 +3814,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="115.153846153846"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.9676113360324"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="116.117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="75.6275303643725"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -3739,15 +3867,14 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="82.502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="67.4331983805668"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.2307692307692"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="68.0202429149798"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -3792,15 +3919,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="78.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="111.910931174089"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="79.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="112.902834008097"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="64.2712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
authorize check service done
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="28"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,6 +38,7 @@
     <sheet name="addAccountContactAffiliations" sheetId="28" state="visible" r:id="rId29"/>
     <sheet name="insertUser" sheetId="29" state="visible" r:id="rId30"/>
     <sheet name="updateUser" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="getRoleActions" sheetId="31" state="visible" r:id="rId32"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="150">
   <si>
     <t>URL</t>
   </si>
@@ -60,7 +61,7 @@
     <t>SchemaPath</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authentication/authentication/deactivateUserLogins</t>
+    <t>/web-corporate/api/submit/authentication/authentication/deactivateUserLogins</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{"UserNames":["aaa@bss.com"]}}</t>
@@ -69,13 +70,13 @@
     <t>jsonSchema/authentication/authentication/deactivateUserLogins.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authentication/authentication/activateUserLogins</t>
+    <t>/web-corporate/api/submit/authentication/authentication/activateUserLogins</t>
   </si>
   <si>
     <t>jsonSchema/authentication/authentication/activateUserLogins.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/authentication/getAuthenticatedUser</t>
+    <t>/web-corporate/authentication/getAuthenticatedUser</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{}}</t>
@@ -324,7 +325,7 @@
     <t>/authorize/setupService/relateUsersToRole</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/authentication/login</t>
+    <t>/web-corporate/authentication/login</t>
   </si>
   <si>
     <t>{"Header": {},"Params": {"UserName": "anik","Password": "12345678"}}</t>
@@ -336,7 +337,7 @@
     <t>{"Header": {},"Params": {"UserName": "ntm","Password": "12345678"}}</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/authentication/logout</t>
+    <t>/web-corporate/authentication/logout</t>
   </si>
   <si>
     <t>{"Header": {},"Params": {}}</t>
@@ -345,7 +346,7 @@
     <t>jsonSchema/authentication/logout.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authentication/authentication/requestPasswordReset</t>
+    <t>/web-corporate/api/submit/authentication/authentication/requestPasswordReset</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{"UserName":"aaa@bss.com"}}</t>
@@ -354,7 +355,7 @@
     <t>jsonSchema/authentication/authentication/requestPasswordReset.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/authentication/authentication/verifyPasswordResetToken</t>
+    <t>/web-corporate/authentication/authentication/verifyPasswordResetToken</t>
   </si>
   <si>
     <t>{ "Header": {}, "Params": { "ResetToken": "74Oe1VioEd+elt61qc2HFg=="}}</t>
@@ -363,7 +364,7 @@
     <t>jsonSchema/authentication/authentication/verifyPasswordResetToken.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/authentication/authentication/updatePassword</t>
+    <t>/web-corporate/authentication/authentication/updatePassword</t>
   </si>
   <si>
     <t>{  "Header": {},  "Params":{ "Password": "12345678", "ConfirmPassword": "12345678", "ExistingPassword": "12345678"}}</t>
@@ -385,7 +386,7 @@
     <t>resources/jsonSchema/updatePasswordGuest_pass.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authorize/setup/insertRole</t>
+    <t>/web-corporate/api/submit/authorize/setup/insertRole</t>
   </si>
   <si>
     <t>{
@@ -401,7 +402,7 @@
     <t>resources/jsonSchema/insertRole_pass.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authorize/setup/deleteRole</t>
+    <t>/web-corporate/api/submit/authorize/setup/deleteRole</t>
   </si>
   <si>
     <t>{
@@ -439,7 +440,7 @@
     <t>resources/jsonSchema/deleteRole_fail.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authorize/setup/getRights</t>
+    <t>/web-corporate/api/submit/authorize/setup/getRights</t>
   </si>
   <si>
     <t>{
@@ -453,19 +454,19 @@
     <t>resources/jsonSchema/getRights_pass.json</t>
   </si>
   <si>
-    <t>http://10.0.0.111:8080/web-corporate/api/submit/authorize/check/getUserActions</t>
-  </si>
-  <si>
-    <t>jsonSchema/getUserActions-Pass.json</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/web-corporate/api/submit/authorize/check/getRolesAuthenticatedUser</t>
-  </si>
-  <si>
-    <t>jsonSchema/getRolesAuthenticatedUser-pass.json</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/getAccounts</t>
+    <t>/web-corporate/api/submit/authorize/check/getUserActions</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/check/getUserActions.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authorize/check/getRolesAuthenticatedUser</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/check/getRolesAuthenticatedUser.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/corporate/account/getAccounts</t>
   </si>
   <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"DESC"}]},"Params":{}}</t>
@@ -474,13 +475,13 @@
     <t>jsonSchema/corporate/account/getAccounts.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/insertAccounts</t>
+    <t>/web-corporate/api/submit/corporate/account/insertAccounts</t>
   </si>
   <si>
     <t>jsonSchema/corporate/account/insertAccounts.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/updateAccounts</t>
+    <t>/web-corporate/api/submit/corporate/account/updateAccounts</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{"Accounts":[{"AccountID":38,"oca":1}]}}</t>
@@ -489,7 +490,7 @@
     <t>jsonSchema/corporate/account/updateAccounts.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/deleteAccounts</t>
+    <t>/web-corporate/api/submit/corporate/account/deleteAccounts</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{"AccountIDs": [43}}</t>
@@ -498,7 +499,7 @@
     <t>jsonSchema/corporate/account/deleteAccounts.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/getAccountContacts</t>
+    <t>/web-corporate/api/submit/corporate/account/getAccountContacts</t>
   </si>
   <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"DESC"}]},"Params":{"AcountIDs":[40]}}</t>
@@ -507,7 +508,7 @@
     <t>jsonSchema/corporate/account/getAccountContacts.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/account/addAccountContactAffiliations</t>
+    <t>/web-corporate/api/submit/corporate/account/addAccountContactAffiliations</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{"AccountIDs":[39,40],"ContactIDs":[1,2],"AffiliationTypeIDs":[1,2]}}</t>
@@ -516,16 +517,25 @@
     <t>jsonSchema/corporate/account/addAccountContactAffiliations.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/user/insertUser</t>
+    <t>/web-corporate/api/submit/corporate/user/insertUser</t>
   </si>
   <si>
     <t>jsonSchema/corporate/user/insertUser.json</t>
   </si>
   <si>
-    <t>http://localhost:8080/web-corporate/api/submit/corporate/user/updateUser</t>
+    <t>/web-corporate/api/submit/corporate/user/updateUser</t>
   </si>
   <si>
     <t>jsonSchema/corporate/user/updateUser.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authorize/check/getRoleActions</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"RoleIDs":[13]}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/check/getRoleActions.json</t>
   </si>
 </sst>
 </file>
@@ -537,7 +547,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -603,20 +613,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -738,7 +734,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -855,14 +851,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -874,66 +862,6 @@
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF1155CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -944,16 +872,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.8056680161943"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="86.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.5182186234818"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="68.2348178137652"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,15 +925,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1020,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>104</v>
       </c>
@@ -1049,15 +977,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1072,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>109</v>
       </c>
@@ -1101,15 +1029,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3805668016194"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1124,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
         <v>112</v>
       </c>
@@ -1153,15 +1081,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1216,15 +1144,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1239,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>119</v>
       </c>
@@ -1250,7 +1178,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
         <v>119</v>
       </c>
@@ -1279,7 +1207,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1320,7 +1248,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1359,7 +1287,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1399,7 +1327,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1437,7 +1365,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1475,16 +1403,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.4858299595142"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="87.9433198380567"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="68.2348178137652"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,14 +1456,14 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1566,17 +1494,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.9838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1591,25 +1519,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1631,15 +1548,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1683,15 +1600,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="94.1578947368421"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="96.6194331983806"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1735,15 +1652,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.1619433198381"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1787,15 +1704,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1839,15 +1756,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.2712550607288"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.0890688259109"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1891,15 +1808,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.9838056680162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1943,15 +1860,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="95.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="98.1214574898785"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1995,16 +1912,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.3562753036437"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,13 +1936,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="5" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2047,15 +1964,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2099,16 +2016,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.3562753036437"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,13 +2040,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="5" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2144,6 +2061,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2151,7 +2120,7 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F30" activeCellId="0" sqref="F30"/>
@@ -2159,19 +2128,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -3696,16 +3665,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.9514170040486"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.4898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="65.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="68.2348178137652"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3759,15 +3728,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3782,8 +3751,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -3794,9 +3763,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://localhost:8080/web-corporate/authentication/logout"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3814,15 +3780,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="116.117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="119.331983805668"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -3867,14 +3833,14 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.2307692307692"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="68.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.4817813765182"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="69.7327935222672"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -3919,15 +3885,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="79.1619433198381"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="112.902834008097"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="81.1943319838057"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="115.902834008097"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.8785425101215"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3942,7 +3908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
authorize setup few done
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,6 +39,7 @@
     <sheet name="insertUser" sheetId="29" state="visible" r:id="rId30"/>
     <sheet name="updateUser" sheetId="30" state="visible" r:id="rId31"/>
     <sheet name="getRoleActions" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="getLogicalRoles" sheetId="32" state="visible" r:id="rId33"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="150">
   <si>
     <t>URL</t>
   </si>
@@ -389,55 +390,25 @@
     <t>/web-corporate/api/submit/authorize/setup/insertRole</t>
   </si>
   <si>
-    <t>{
-  "Header": {},
-  "Params":{
-    "Name": "Co-ordinator87",
-    "Description": "Test Description",
-    "LogicalRoles": [1,2,3,4]
-   }
-}</t>
-  </si>
-  <si>
-    <t>resources/jsonSchema/insertRole_pass.json</t>
+    <t>jsonSchema/authorize/setup/insertRole.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authorize/setup/updateRole</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"ID":"30","oca":"1"}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/setup/updateRole.json</t>
   </si>
   <si>
     <t>/web-corporate/api/submit/authorize/setup/deleteRole</t>
   </si>
   <si>
-    <t>{
-  "Header": {},
-  "Params":{
-      "ID": 16,
-      "oca": 1,
-      "Name": "Co-ordinator2"
-   }
-}</t>
-  </si>
-  <si>
-    <t>resources/jsonSchema/updateRole_pass.json</t>
-  </si>
-  <si>
-    <t>{
-  "Header": {},
-  "Params":{
-      "RoleID": 2
-  }
-}</t>
-  </si>
-  <si>
-    <t>resources/jsonSchema/deleteRole_pass.json</t>
-  </si>
-  <si>
-    <t>{
-  "Header": {},
-  "Params":{
-      "RoleID": 16
-  }
-}</t>
-  </si>
-  <si>
-    <t>resources/jsonSchema/deleteRole_fail.json</t>
+    <t>{ "Header": {}, "Params":{"ID": 32}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/setup/deleteRole.json</t>
   </si>
   <si>
     <t>/web-corporate/api/submit/authorize/setup/getRights</t>
@@ -536,6 +507,12 @@
   </si>
   <si>
     <t>jsonSchema/authorize/check/getRoleActions.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authorize/setup/getLogicalRoles</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/setup/getLogicalRoles.json</t>
   </si>
 </sst>
 </file>
@@ -878,10 +855,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="86.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.5182186234818"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="68.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="70.7004048582996"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,9 +908,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.2348178137652"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -978,14 +955,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="59.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1000,15 +977,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="25" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1030,14 +1007,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1052,15 +1029,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1081,15 +1058,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1104,9 +1081,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>115</v>
@@ -1115,17 +1092,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>118</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1150,9 +1117,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1169,24 +1136,24 @@
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1409,10 +1376,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="87.9433198380567"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.0931174089069"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="68.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="70.7004048582996"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,7 +1430,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1496,15 +1463,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1521,13 +1488,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1554,9 +1521,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.4089068825911"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1573,13 +1540,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1606,9 +1573,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="96.6194331983806"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="100.048582995951"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1625,13 +1592,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1658,9 +1625,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1677,13 +1644,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1710,9 +1677,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1729,13 +1696,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1762,9 +1729,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.0890688259109"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.7692307692308"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1781,13 +1748,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1814,9 +1781,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.9838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.6599190283401"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1833,13 +1800,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1866,9 +1833,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="98.1214574898785"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="101.550607287449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1885,13 +1852,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1918,9 +1885,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="69.412955465587"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="72.5182186234818"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1937,13 +1904,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1970,9 +1937,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2022,9 +1989,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="69.412955465587"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="72.5182186234818"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2041,13 +2008,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2074,9 +2041,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2093,10 +2060,62 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>147</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="B2" s="5" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>149</v>
@@ -2128,19 +2147,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -3671,10 +3690,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="65.663967611336"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="68.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.0202429149798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="70.7004048582996"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3734,9 +3753,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3786,9 +3805,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="119.331983805668"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="123.615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.3400809716599"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -3839,8 +3858,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="69.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="88.5870445344129"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="72.0890688259109"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -3891,9 +3910,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="81.1943319838057"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="115.902834008097"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.0890688259109"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="120.080971659919"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.2348178137652"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
authorize setup add remove rights done
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="155">
   <si>
     <t>URL</t>
   </si>
@@ -423,6 +423,21 @@
   </si>
   <si>
     <t>resources/jsonSchema/getRights_pass.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authorize/setup/addRightsToRole</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"RoleIDs":[29,30],"ActionIDs":[98,99]}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/setup/addRightsToRole.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authorize/setup/removeRightsFromRole</t>
+  </si>
+  <si>
+    <t>jsonSchema/authorize/setup/removeRightsFromRole.json</t>
   </si>
   <si>
     <t>/web-corporate/api/submit/authorize/check/getUserActions</t>
@@ -855,10 +870,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="82.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="90.7287449392713"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="71.2348178137652"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,9 +923,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -960,9 +975,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.2388663967611"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="59.9878542510121"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1012,9 +1027,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1058,15 +1073,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.3441295546559"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.7732793522267"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1117,9 +1132,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1252,16 +1267,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="55.8947368421053"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="46.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1274,6 +1290,17 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1292,15 +1319,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="60.085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="57.5506072874494"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="47.2955465587045"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,6 +1342,17 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1376,10 +1417,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="82.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="71.2348178137652"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,7 +1471,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1469,9 +1510,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1488,13 +1529,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1521,9 +1562,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.4089068825911"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="85.1578947368421"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1540,13 +1581,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1573,9 +1614,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="74.9838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="100.048582995951"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="100.906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1592,13 +1633,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1625,9 +1666,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="76.3765182186235"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1644,13 +1685,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1677,9 +1718,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1696,13 +1737,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1729,9 +1770,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.7692307692308"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="78.412955465587"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1748,13 +1789,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1781,9 +1822,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.6599190283401"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.4089068825911"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="55.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1800,13 +1841,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1833,9 +1874,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="101.550607287449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.7287449392713"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="102.404858299595"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.8785425101215"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1852,13 +1893,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1885,9 +1926,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="69.412955465587"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.0566801619433"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="73.1619433198381"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1904,13 +1945,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1937,9 +1978,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.7287449392713"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.8785425101215"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1989,9 +2030,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="69.412955465587"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.0566801619433"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="73.1619433198381"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2008,13 +2049,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2041,9 +2082,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2060,13 +2101,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2093,9 +2134,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2112,13 +2153,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2147,19 +2188,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -3690,10 +3731,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.0202429149798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="82.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="70.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.5546558704453"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="71.2348178137652"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,9 +3794,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3805,9 +3846,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="123.615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="124.793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.9838056680162"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -3858,8 +3899,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="88.5870445344129"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="72.7327935222672"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -3910,9 +3951,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.0890688259109"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="120.080971659919"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="121.14979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
authentication default diff senario added
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="159">
   <si>
     <t>URL</t>
   </si>
@@ -86,6 +86,9 @@
     <t>jsonSchema/authentication/getAuthenticatedUser.json</t>
   </si>
   <si>
+    <t>jsonSchema/authentication/getAuthenticatedUserAfterLogin.json</t>
+  </si>
+  <si>
     <t>Api</t>
   </si>
   <si>
@@ -338,10 +341,19 @@
     <t>{"Header": {},"Params": {"UserName": "ntm","Password": "12345678"}}</t>
   </si>
   <si>
+    <t>{"Header": {},"Params": {"UserName": "anik2","Password": "12345678"}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/login_failed_invalid_user_or_pass.json</t>
+  </si>
+  <si>
+    <t>{"Header": {},"Params": {}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/login_invalid_request_format.json</t>
+  </si>
+  <si>
     <t>/web-corporate/authentication/logout</t>
-  </si>
-  <si>
-    <t>{"Header": {},"Params": {}}</t>
   </si>
   <si>
     <t>jsonSchema/authentication/logout.json</t>
@@ -865,15 +877,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="90.7287449392713"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="83.1255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="95.6558704453441"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="76.3765182186235"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="74.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,14 +930,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -942,13 +954,13 @@
     </row>
     <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -970,14 +982,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A5 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.5951417004049"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="63.7368421052632"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -994,13 +1006,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1022,14 +1034,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A5 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1046,13 +1058,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1074,14 +1086,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A5 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.7044534412956"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1098,13 +1110,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1127,14 +1139,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A5 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1151,24 +1163,24 @@
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1202,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1231,7 +1243,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="A5 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1270,14 +1282,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="56.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="55.8947368421053"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="46.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="58.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1294,13 +1306,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1321,15 +1333,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A5 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="60.085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="57.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="47.2955465587045"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="63.1983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="60.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1346,13 +1358,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1386,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1412,15 +1424,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="83.1255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.0890688259109"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="96.7287449392713"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="74.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,13 +1477,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1505,14 +1517,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A5 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.6923076923077"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1529,13 +1541,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1557,14 +1569,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="85.1578947368421"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.6599190283401"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1581,13 +1593,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1609,14 +1621,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="100.906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="106.477732793522"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1633,13 +1645,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1661,14 +1673,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="76.3765182186235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.3400809716599"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1685,13 +1697,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1713,14 +1725,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1737,13 +1749,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1765,14 +1777,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="78.412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="82.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1789,13 +1801,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1817,14 +1829,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="1" sqref="A5 B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.4089068825911"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="85.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1841,13 +1853,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1869,14 +1881,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.7287449392713"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="102.404858299595"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.6558704453441"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="107.975708502024"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1893,13 +1905,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1921,14 +1933,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.6963562753036"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="77.0202429149798"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1945,13 +1957,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1970,17 +1982,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A5 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.7287449392713"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.8785425101215"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.6558704453441"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2004,6 +2016,17 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2025,14 +2048,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.6963562753036"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="77.0202429149798"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2049,13 +2072,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2077,14 +2100,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.6923076923077"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2101,13 +2124,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2129,14 +2152,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2153,13 +2176,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2183,43 +2206,43 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topRight" activeCell="F30" activeCellId="1" sqref="A5 F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -2231,69 +2254,69 @@
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="n">
@@ -2307,25 +2330,25 @@
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>12345678</v>
@@ -2340,117 +2363,117 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L7" s="15" t="n">
         <v>8</v>
@@ -2461,34 +2484,34 @@
     </row>
     <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="n">
@@ -2500,31 +2523,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J9" s="12" t="n">
         <v>12345678</v>
@@ -2541,25 +2564,25 @@
       <c r="A10" s="11"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J10" s="20" t="n">
         <v>12345678</v>
@@ -2576,31 +2599,31 @@
       <c r="A11" s="11"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J11" s="20" t="n">
         <v>12345678</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L11" s="20" t="n">
         <v>8</v>
@@ -2613,31 +2636,31 @@
       <c r="A12" s="11"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12" s="15" t="n">
         <v>32</v>
@@ -2648,57 +2671,57 @@
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E14" s="12" t="n">
         <v>1000</v>
@@ -2707,35 +2730,35 @@
         <v>-1</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="J14" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="20" t="n">
         <v>0</v>
@@ -2744,165 +2767,165 @@
         <v>0</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J16" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J18" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L19" s="15" t="n">
         <v>8</v>
@@ -2913,429 +2936,429 @@
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J24" s="20" t="n">
         <v>10</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="17"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J25" s="20" t="n">
         <v>2</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J26" s="20"/>
       <c r="K26" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M26" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H29" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="22" t="s">
         <v>54</v>
-      </c>
-      <c r="I29" s="22" t="s">
-        <v>53</v>
       </c>
       <c r="J29" s="22" t="n">
         <v>1</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M30" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E31" s="12" t="n">
         <v>1000</v>
@@ -3344,33 +3367,33 @@
         <v>-1</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E32" s="20" t="n">
         <v>0</v>
@@ -3379,7 +3402,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
@@ -3392,19 +3415,19 @@
       <c r="A33" s="11"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -3415,16 +3438,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" s="12" t="n">
         <v>1000</v>
@@ -3433,19 +3456,19 @@
         <v>-1</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L34" s="12"/>
       <c r="M34" s="14"/>
@@ -3454,10 +3477,10 @@
       <c r="A35" s="11"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" s="20" t="n">
         <v>0</v>
@@ -3466,19 +3489,19 @@
         <v>0</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L35" s="20" t="n">
         <v>8</v>
@@ -3491,31 +3514,31 @@
       <c r="A36" s="11"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="21"/>
@@ -3529,57 +3552,57 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L37" s="15"/>
       <c r="M37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="J38" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3591,13 +3614,13 @@
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
@@ -3612,13 +3635,13 @@
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
@@ -3626,41 +3649,41 @@
     </row>
     <row r="41" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="J41" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M41" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,20 +3695,20 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3723,18 +3746,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.5546558704453"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="83.1255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="74.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3750,26 +3773,49 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3789,14 +3835,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="55.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3813,13 +3859,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3841,14 +3887,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="124.793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.4858299595142"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="131.647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="85.3724696356275"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -3866,13 +3912,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3894,13 +3940,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="72.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="94.1578947368421"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="76.6963562753036"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -3918,13 +3964,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3946,14 +3992,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.8380566801619"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="121.14979757085"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.7692307692308"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.4453441295547"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="127.793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.5182186234818"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3970,13 +4016,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few senario added password
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,41 +5,42 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="activateUserLogins" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="getAuthenticatedUser" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="API Request Matrix" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="login" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="logout" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="requestPasswordReset" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="verifyPasswordResetToken" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="updatePassword" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="updatePasswordGuest" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="insertRole" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="updateRole" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="deleteRole" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="getRights" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="getRoleUsers" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="getUsers" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="addRightsToRole" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="removeRightsFromRole" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="addUsersToRole" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="removeUsersFromRole" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="getUserActions" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="getRolesAuthenticatedUser" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="getAccounts" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="insertAccounts" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="updateAccounts" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="deleteAccounts" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="getAccountContacts" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="addAccountContactAffiliations" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="insertUser" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="updateUser" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="getRoleActions" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="getLogicalRoles" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="login_failed" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="login" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="logout" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="requestPasswordReset" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="verifyPasswordResetToken" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="updatePassword" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="updatePasswordGuest" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="insertRole" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="updateRole" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="deleteRole" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="getRights" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="getRoleUsers" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="getUsers" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="addRightsToRole" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="removeRightsFromRole" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="addUsersToRole" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="removeUsersFromRole" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="getUserActions" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="getRolesAuthenticatedUser" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="getAccounts" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="insertAccounts" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="updateAccounts" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="deleteAccounts" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="getAccountContacts" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="addAccountContactAffiliations" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="insertUser" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="updateUser" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="getRoleActions" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="getLogicalRoles" sheetId="33" state="visible" r:id="rId34"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="170">
   <si>
     <t>URL</t>
   </si>
@@ -332,6 +333,18 @@
     <t>/web-corporate/authentication/login</t>
   </si>
   <si>
+    <t>{"Header": {},"Params": {"UserName": "anik2","Password": "12345678"}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/login_failed_invalid_user_or_pass.json</t>
+  </si>
+  <si>
+    <t>{"Header": {},"Params": {}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/login_invalid_request_format.json</t>
+  </si>
+  <si>
     <t>{"Header": {},"Params": {"UserName": "anik","Password": "12345678"}}</t>
   </si>
   <si>
@@ -341,18 +354,6 @@
     <t>{"Header": {},"Params": {"UserName": "ntm","Password": "12345678"}}</t>
   </si>
   <si>
-    <t>{"Header": {},"Params": {"UserName": "anik2","Password": "12345678"}}</t>
-  </si>
-  <si>
-    <t>jsonSchema/authentication/login_failed_invalid_user_or_pass.json</t>
-  </si>
-  <si>
-    <t>{"Header": {},"Params": {}}</t>
-  </si>
-  <si>
-    <t>jsonSchema/authentication/login_invalid_request_format.json</t>
-  </si>
-  <si>
     <t>/web-corporate/authentication/logout</t>
   </si>
   <si>
@@ -368,7 +369,16 @@
     <t>jsonSchema/authentication/authentication/requestPasswordReset.json</t>
   </si>
   <si>
-    <t>/web-corporate/authentication/authentication/verifyPasswordResetToken</t>
+    <t>{"Header":{},"Params":{"UserName":"invalid"}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/authentication/requestPasswordReset_invalidUser.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/authentication/requestPasswordReset_invalidParam.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authentication/authentication/verifyPasswordResetToken</t>
   </si>
   <si>
     <t>{ "Header": {}, "Params": { "ResetToken": "74Oe1VioEd+elt61qc2HFg=="}}</t>
@@ -377,13 +387,37 @@
     <t>jsonSchema/authentication/authentication/verifyPasswordResetToken.json</t>
   </si>
   <si>
-    <t>/web-corporate/authentication/authentication/updatePassword</t>
+    <t>{ "Header": {}, "Params": { "ResetToken": "invalid"}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/authentication/verifyPasswordResetTokenInvalidToken.json</t>
+  </si>
+  <si>
+    <t>{ "Header": {}, "Params": {}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/authentication/verifyPasswordResetTokenInvalidParam.json</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/authentication/authentication/updatePassword</t>
   </si>
   <si>
     <t>{  "Header": {},  "Params":{ "Password": "12345678", "ConfirmPassword": "12345678", "ExistingPassword": "12345678"}}</t>
   </si>
   <si>
     <t>jsonSchema/authentication/authentication/updatePassword.json</t>
+  </si>
+  <si>
+    <t>{  "Header": {},  "Params":{ "Password": "112", "ConfirmPassword": "12", "ExistingPassword": "12"}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/authentication/updatePasswordInvalidPass.json</t>
+  </si>
+  <si>
+    <t>{  "Header": {},  "Params":{ }}</t>
+  </si>
+  <si>
+    <t>jsonSchema/authentication/authentication/updatePasswordInvalidParam.json</t>
   </si>
   <si>
     <t>{
@@ -876,16 +910,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="95.6558704453441"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.6234817813765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="76.3765182186235"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="98.2267206477733"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="78.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,17 +961,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.5627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="69.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="131.327935222672"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.3400809716599"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -952,15 +986,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -981,16 +1037,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A5 C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="49.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,24 +1060,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="25" t="n">
+        <v>115</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -1033,19 +1089,19 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A5 C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.7732793522267"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
-    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1057,14 +1113,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>117</v>
+      <c r="A2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="25" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1083,17 +1139,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A5 B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1109,17 +1165,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>118</v>
+      <c r="A2" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1138,19 +1193,19 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A5 A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.5587044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1161,35 +1216,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>121</v>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
+        <v>129</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1199,29 +1244,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1242,14 +1309,16 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="A5 B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="4.39271255060729"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="6.53441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,18 +1348,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5 A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="59.3441295546559"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="58.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.0607287449393"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,17 +1369,6 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1333,15 +1389,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A5 C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="63.1983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="60.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="50.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1356,15 +1412,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1383,15 +1439,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="64.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,6 +1462,17 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1423,16 +1493,16 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="96.7287449392713"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.6234817813765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="75.9473684210526"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="99.2995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,15 +1546,13 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,18 +1582,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A5 B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.6923076923077"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,17 +1604,6 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1568,16 +1624,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.6599190283401"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.1578947368421"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,13 +1649,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1620,19 +1676,19 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="106.477732793522"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="92.0161943319838"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1645,22 +1701,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -1672,15 +1728,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="80.3400809716599"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="109.368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1697,13 +1753,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>123</v>
+        <v>144</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1724,15 +1780,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="70.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1749,13 +1805,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>139</v>
+        <v>147</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1776,15 +1832,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="82.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="70.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1801,13 +1857,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1828,15 +1884,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="1" sqref="A5 B29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="85.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="70.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1853,13 +1909,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1880,15 +1936,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.6558704453441"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="107.975708502024"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="87.9433198380567"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1905,13 +1961,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1932,15 +1988,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="98.2267206477733"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="110.866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.7004048582996"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1957,13 +2013,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>123</v>
+        <v>158</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1984,15 +2040,15 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A5 C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.6558704453441"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="98.2267206477733"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.7004048582996"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2047,15 +2103,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="79.0526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2072,13 +2128,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2099,15 +2155,67 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5 A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.6923076923077"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.1578947368421"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2124,13 +2232,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2144,22 +2252,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5 A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="55.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2176,13 +2284,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2203,27 +2311,27 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F30" activeCellId="1" sqref="A5 F30"/>
+      <selection pane="topRight" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -3746,18 +3854,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="72.0890688259109"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.6234817813765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.0566801619433"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.0202429149798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,7 +3879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
@@ -3782,7 +3890,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>92</v>
       </c>
@@ -3790,31 +3898,11 @@
         <v>95</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3832,18 +3920,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.0202429149798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3858,16 +3946,30 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3886,39 +3988,38 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="131.647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.4858299595142"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="85.3724696356275"/>
-    <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3937,39 +4038,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="94.1578947368421"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="76.6963562753036"/>
-    <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="67.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3989,18 +4113,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A5 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.4453441295547"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="127.793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="96.6194331983806"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="78.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4015,7 +4139,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -4023,6 +4147,28 @@
       </c>
       <c r="C2" s="4" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few more senario added
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="175">
   <si>
     <t>URL</t>
   </si>
@@ -72,10 +72,22 @@
     <t>jsonSchema/authentication/authentication/deactivateUserLogins.json</t>
   </si>
   <si>
+    <t>{"Header":{},"Params":{}</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"UserNames":["aaaw2@b323ss.com"]}}</t>
+  </si>
+  <si>
     <t>/web-corporate/api/submit/authentication/authentication/activateUserLogins</t>
   </si>
   <si>
     <t>jsonSchema/authentication/authentication/activateUserLogins.json</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"UserNames":["aaa@bss.com2"]}}</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"UserNames":["test"]}}</t>
   </si>
   <si>
     <t>/web-corporate/authentication/getAuthenticatedUser</t>
@@ -478,6 +490,9 @@
   </si>
   <si>
     <t>jsonSchema/authorize/setup/addRightsToRole.json</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"RoleIDs":[1],"ActionIDs":[1]}}</t>
   </si>
   <si>
     <t>/web-corporate/api/submit/authorize/setup/removeRightsFromRole</t>
@@ -908,18 +923,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="98.2267206477733"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="100.797570850202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,7 +959,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -963,15 +1010,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="131.327935222672"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="94.2631578947368"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="134.971659919028"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="76.3765182186235"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -988,35 +1035,35 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1043,9 +1090,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1062,13 +1109,13 @@
     </row>
     <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1095,9 +1142,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.0607287449393"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1114,13 +1161,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1147,9 +1194,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1166,13 +1213,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1199,9 +1246,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1218,13 +1265,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1252,9 +1299,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1271,24 +1318,24 @@
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1387,17 +1434,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="60.9514170040486"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="60.3076923076923"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="61.8056680161943"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1414,13 +1461,35 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1447,9 +1516,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="64.8056680161943"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.1295546558704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="66.412955465587"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.3805668016194"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1466,13 +1535,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1491,18 +1560,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="99.2995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.9838056680162"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="101.975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.0161943319838"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,16 +1587,48 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1591,7 +1692,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1630,9 +1731,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.1578947368421"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="96.6194331983806"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1649,13 +1750,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1682,9 +1783,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="92.0161943319838"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.4777327935223"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1701,13 +1802,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1734,9 +1835,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="109.368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="112.368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1753,13 +1854,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1786,9 +1887,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.6234817813765"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1805,13 +1906,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1838,9 +1939,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.1295546558704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1857,13 +1958,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1890,9 +1991,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.8380566801619"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.1295546558704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="87.0890688259109"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1909,13 +2010,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1942,9 +2043,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="87.9433198380567"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="71.8785425101215"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.1943319838057"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1961,13 +2062,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1994,9 +2095,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="98.2267206477733"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="110.866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="100.797570850202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="113.761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2013,13 +2114,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2046,9 +2147,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="98.2267206477733"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="100.797570850202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2065,24 +2166,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2101,17 +2202,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.6599190283401"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="80.9838056680162"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2128,13 +2229,46 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2161,9 +2295,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.6599190283401"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="80.9838056680162"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2180,13 +2314,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2213,9 +2347,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.1578947368421"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="96.6194331983806"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2232,13 +2366,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2265,9 +2399,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="56.5587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2284,13 +2418,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2319,38 +2453,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -2362,69 +2496,69 @@
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="n">
@@ -2438,25 +2572,25 @@
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>12345678</v>
@@ -2471,117 +2605,117 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L7" s="15" t="n">
         <v>8</v>
@@ -2592,34 +2726,34 @@
     </row>
     <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="n">
@@ -2631,31 +2765,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J9" s="12" t="n">
         <v>12345678</v>
@@ -2672,25 +2806,25 @@
       <c r="A10" s="11"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J10" s="20" t="n">
         <v>12345678</v>
@@ -2707,31 +2841,31 @@
       <c r="A11" s="11"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J11" s="20" t="n">
         <v>12345678</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="L11" s="20" t="n">
         <v>8</v>
@@ -2744,31 +2878,31 @@
       <c r="A12" s="11"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L12" s="15" t="n">
         <v>32</v>
@@ -2779,57 +2913,57 @@
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E14" s="12" t="n">
         <v>1000</v>
@@ -2838,35 +2972,35 @@
         <v>-1</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J14" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E15" s="20" t="n">
         <v>0</v>
@@ -2875,165 +3009,165 @@
         <v>0</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J16" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J18" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L19" s="15" t="n">
         <v>8</v>
@@ -3044,429 +3178,429 @@
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="J21" s="12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J24" s="20" t="n">
         <v>10</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="17"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J25" s="20" t="n">
         <v>2</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J26" s="20"/>
       <c r="K26" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M26" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J29" s="22" t="n">
         <v>1</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M30" s="23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E31" s="12" t="n">
         <v>1000</v>
@@ -3475,33 +3609,33 @@
         <v>-1</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E32" s="20" t="n">
         <v>0</v>
@@ -3510,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
@@ -3523,19 +3657,19 @@
       <c r="A33" s="11"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -3546,16 +3680,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E34" s="12" t="n">
         <v>1000</v>
@@ -3564,19 +3698,19 @@
         <v>-1</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L34" s="12"/>
       <c r="M34" s="14"/>
@@ -3585,10 +3719,10 @@
       <c r="A35" s="11"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E35" s="20" t="n">
         <v>0</v>
@@ -3597,19 +3731,19 @@
         <v>0</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L35" s="20" t="n">
         <v>8</v>
@@ -3622,31 +3756,31 @@
       <c r="A36" s="11"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="K36" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="I36" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="K36" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="21"/>
@@ -3660,57 +3794,57 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L37" s="15"/>
       <c r="M37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J38" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3722,13 +3856,13 @@
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
@@ -3743,13 +3877,13 @@
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
@@ -3757,41 +3891,41 @@
     </row>
     <row r="41" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="D41" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J41" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M41" s="14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3803,20 +3937,20 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3862,10 +3996,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.0202429149798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.9838056680162"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3881,24 +4015,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3928,10 +4062,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.0202429149798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="89.9797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.9838056680162"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3947,24 +4081,24 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3994,9 +4128,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4013,13 +4147,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4046,9 +4180,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="67.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="87.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="69.412955465587"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="89.9797570850202"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -4066,35 +4200,35 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -4121,8 +4255,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="96.6194331983806"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="78.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="99.1902834008097"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="80.6599190283401"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -4140,35 +4274,35 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cookie befor each call
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="174">
   <si>
     <t>URL</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>{"Header":{},"Params":{}}</t>
-  </si>
-  <si>
-    <t>jsonSchema/authentication/getAuthenticatedUser.json</t>
   </si>
   <si>
     <t>jsonSchema/authentication/getAuthenticatedUserAfterLogin.json</t>
@@ -931,10 +928,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="100.797570850202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.3400809716599"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="101.655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,9 +1013,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="94.2631578947368"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="134.971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="76.3765182186235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="95.0161943319838"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="136.255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.0202429149798"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1035,35 +1032,35 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1090,9 +1087,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="83.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.6234817813765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.6963562753036"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1109,13 +1106,13 @@
     </row>
     <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1142,9 +1139,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.5951417004049"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.7004048582996"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1161,13 +1158,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1194,9 +1191,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1213,13 +1210,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>131</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1246,9 +1243,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.1295546558704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1265,13 +1262,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>134</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1299,9 +1296,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1318,24 +1315,24 @@
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1436,15 +1433,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="62.4493927125506"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="61.8056680161943"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1461,35 +1458,35 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1516,9 +1513,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="66.412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1535,13 +1532,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1568,10 +1565,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="101.975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.0161943319838"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="102.939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1689,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1731,9 +1728,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="96.6194331983806"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="97.4777327935223"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1750,13 +1747,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1783,9 +1780,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.4777327935223"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.2267206477733"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1802,13 +1799,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1835,9 +1832,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="112.368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.6234817813765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="113.331983805668"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1854,13 +1851,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1887,9 +1884,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="85.3724696356275"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1906,13 +1903,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1939,9 +1936,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="58.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1958,13 +1955,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1991,9 +1988,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="87.0890688259109"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="87.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="58.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2010,13 +2007,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2043,9 +2040,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.1943319838057"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="61.4858299595142"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2062,13 +2059,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2095,9 +2092,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="100.797570850202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="113.761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="101.655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="114.82995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2114,13 +2111,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2139,17 +2136,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="100.797570850202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="101.655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2173,17 +2170,6 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2210,9 +2196,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="78.3036437246964"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="81.7327935222672"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2229,46 +2215,46 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2295,9 +2281,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="78.3036437246964"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="81.7327935222672"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2314,13 +2300,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2347,9 +2333,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="96.6194331983806"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="97.4777327935223"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2366,13 +2352,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2399,9 +2385,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="58.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2418,13 +2404,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2453,38 +2439,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -2496,69 +2482,69 @@
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>32</v>
-      </c>
       <c r="C3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="n">
@@ -2572,25 +2558,25 @@
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>12345678</v>
@@ -2605,117 +2591,117 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="I5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="L7" s="15" t="n">
         <v>8</v>
@@ -2726,34 +2712,34 @@
     </row>
     <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="J8" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="n">
@@ -2765,31 +2751,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" s="12" t="n">
         <v>12345678</v>
@@ -2806,25 +2792,25 @@
       <c r="A10" s="11"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="20" t="n">
         <v>12345678</v>
@@ -2841,31 +2827,31 @@
       <c r="A11" s="11"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="20" t="n">
         <v>12345678</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11" s="20" t="n">
         <v>8</v>
@@ -2878,31 +2864,31 @@
       <c r="A12" s="11"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="L12" s="15" t="n">
         <v>32</v>
@@ -2913,57 +2899,57 @@
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="E14" s="12" t="n">
         <v>1000</v>
@@ -2972,35 +2958,35 @@
         <v>-1</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J14" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="20" t="n">
         <v>0</v>
@@ -3009,165 +2995,165 @@
         <v>0</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>63</v>
-      </c>
       <c r="K15" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="E16" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="F16" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="I16" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="15" t="s">
+      <c r="I19" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="J19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="15" t="s">
-        <v>36</v>
-      </c>
       <c r="K19" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L19" s="15" t="n">
         <v>8</v>
@@ -3178,429 +3164,429 @@
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="12" t="s">
+      <c r="I21" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H23" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="I23" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>76</v>
-      </c>
       <c r="K23" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>78</v>
-      </c>
       <c r="I24" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J24" s="20" t="n">
         <v>10</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="17"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J25" s="20" t="n">
         <v>2</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J26" s="20"/>
       <c r="K26" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M26" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H28" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="I28" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>76</v>
-      </c>
       <c r="K28" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J29" s="22" t="n">
         <v>1</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="22" t="s">
-        <v>82</v>
-      </c>
       <c r="I30" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M30" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="E31" s="12" t="n">
         <v>1000</v>
@@ -3609,33 +3595,33 @@
         <v>-1</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="20" t="n">
         <v>0</v>
@@ -3644,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
@@ -3657,19 +3643,19 @@
       <c r="A33" s="11"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="E33" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>66</v>
-      </c>
       <c r="F33" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -3680,16 +3666,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="E34" s="12" t="n">
         <v>1000</v>
@@ -3698,19 +3684,19 @@
         <v>-1</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L34" s="12"/>
       <c r="M34" s="14"/>
@@ -3719,10 +3705,10 @@
       <c r="A35" s="11"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E35" s="20" t="n">
         <v>0</v>
@@ -3731,19 +3717,19 @@
         <v>0</v>
       </c>
       <c r="G35" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="I35" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="J35" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J35" s="20" t="s">
-        <v>36</v>
-      </c>
       <c r="K35" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L35" s="20" t="n">
         <v>8</v>
@@ -3756,31 +3742,31 @@
       <c r="A36" s="11"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="E36" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>66</v>
-      </c>
       <c r="F36" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H36" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I36" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>87</v>
-      </c>
       <c r="K36" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="21"/>
@@ -3794,57 +3780,57 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="K37" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L37" s="15"/>
       <c r="M37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="D38" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="F38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="I38" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J38" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3856,13 +3842,13 @@
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
@@ -3877,13 +3863,13 @@
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
@@ -3891,41 +3877,41 @@
     </row>
     <row r="41" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="F41" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H41" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="I41" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J41" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M41" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,20 +3923,20 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3996,10 +3982,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4015,24 +4001,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4057,15 +4043,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4081,24 +4067,24 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4128,9 +4114,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="60.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4147,13 +4133,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4180,9 +4166,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="69.412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.4898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="70.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="90.8380566801619"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
@@ -4200,35 +4186,35 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>107</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4255,8 +4241,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="99.1902834008097"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="80.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="100.048582995951"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="81.4089068825911"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -4274,35 +4260,35 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
authentication default all done
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,42 +5,43 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="activateUserLogins" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="getAuthenticatedUser" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="API Request Matrix" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="login_failed" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="login" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="logout" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="requestPasswordReset" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="verifyPasswordResetToken" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="updatePassword" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="updatePasswordGuest" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="insertRole" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="updateRole" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="deleteRole" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="getRights" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="getRoleUsers" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="getUsers" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="addRightsToRole" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="removeRightsFromRole" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="addUsersToRole" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="removeUsersFromRole" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="getUserActions" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="getRolesAuthenticatedUser" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="getAccounts" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="insertAccounts" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="updateAccounts" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="deleteAccounts" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="getAccountContacts" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="addAccountContactAffiliations" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="insertUser" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="updateUser" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="getRoleActions" sheetId="32" state="visible" r:id="rId33"/>
-    <sheet name="getLogicalRoles" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="getAuthenticatedUserLogout" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="getAuthenticatedUser" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="API Request Matrix" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="login_failed" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="login" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="logout" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="requestPasswordReset" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="verifyPasswordResetToken" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="updatePassword" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="updatePasswordGuest" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="insertRole" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="updateRole" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="deleteRole" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="getRights" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="getRoleUsers" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="getUsers" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="addRightsToRole" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="removeRightsFromRole" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="addUsersToRole" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="removeUsersFromRole" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="getUserActions" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="getRolesAuthenticatedUser" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="getAccounts" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="insertAccounts" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="updateAccounts" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="deleteAccounts" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="getAccountContacts" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="addAccountContactAffiliations" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="insertUser" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="updateUser" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="getRoleActions" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="getLogicalRoles" sheetId="34" state="visible" r:id="rId35"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="176">
   <si>
     <t>URL</t>
   </si>
@@ -96,6 +97,9 @@
     <t>{"Header":{},"Params":{}}</t>
   </si>
   <si>
+    <t>jsonSchema/authentication/getAuthenticatedUser.json</t>
+  </si>
+  <si>
     <t>jsonSchema/authentication/getAuthenticatedUserAfterLogin.json</t>
   </si>
   <si>
@@ -361,6 +365,9 @@
   </si>
   <si>
     <t>{"Header": {},"Params": {"UserName": "ntm","Password": "12345678"}}</t>
+  </si>
+  <si>
+    <t>{"Header": {},"Params": {"UserName": "ntm","Password": "123"}}</t>
   </si>
   <si>
     <t>/web-corporate/authentication/logout</t>
@@ -928,10 +935,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="101.655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.9838056680162"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="103.582995951417"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="94.9068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="80.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,15 +1015,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="95.0161943319838"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="136.255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.0202429149798"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="101.761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="82.8016194331984"/>
+    <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,36 +1038,36 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1079,17 +1086,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.6234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="96.7287449392713"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="138.720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="78.3036437246964"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1104,14 +1111,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1134,15 +1163,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="67.7004048582996"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,12 +1185,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="B2" s="25" t="n">
-        <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>128</v>
@@ -1169,11 +1198,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -1191,13 +1220,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.9514170040486"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="68.7692307692308"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
-    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1209,14 +1238,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="25" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1235,17 +1264,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.5587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="47.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1261,17 +1290,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1291,14 +1319,67 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1315,24 +1396,24 @@
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1346,7 +1427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1387,7 +1468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1426,7 +1507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1439,82 +1520,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="51.9514170040486"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="64.2712550607287"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="63.412955465587"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="52.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
@@ -1530,15 +1537,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>143</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1565,10 +1594,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="102.939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.6599190283401"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="104.655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="94.9068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="82.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="80.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,15 +1671,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="68.2348178137652"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,6 +1694,17 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1688,9 +1731,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,18 +1761,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="97.4777327935223"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,17 +1783,6 @@
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1775,15 +1804,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.2267206477733"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="99.1902834008097"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,15 +1859,15 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="84.6234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="113.331983805668"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="96.9433198380567"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1854,19 +1883,19 @@
         <v>148</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -1884,9 +1913,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="85.3724696356275"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="115.368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1903,10 +1932,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>152</v>
@@ -1937,8 +1966,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="86.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1957,11 +1986,11 @@
       <c r="A2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1988,9 +2017,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="87.8380566801619"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="88.4817813765182"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2007,13 +2036,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2035,14 +2064,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="61.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.4453441295547"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="59.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2059,13 +2088,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2087,14 +2116,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="101.655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="114.82995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="92.5506072874494"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.4493927125506"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2111,13 +2140,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2138,15 +2167,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="101.655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="103.582995951417"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="68.1295546558705"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2188,17 +2217,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="103.582995951417"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="116.761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="68.1295546558705"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2215,45 +2244,12 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>123</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="C5" s="5" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2273,17 +2269,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="78.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="79.6963562753036"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="83.1255060728745"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2306,6 +2302,39 @@
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2328,18 +2357,18 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="97.4777327935223"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2354,20 +2383,20 @@
       <c r="A2" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2380,14 +2409,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="99.1902834008097"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2404,13 +2433,65 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>172</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2429,6 +2510,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="103.582995951417"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="68.1295546558705"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2439,38 +2572,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -2482,69 +2615,69 @@
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="n">
@@ -2558,25 +2691,25 @@
       <c r="A4" s="11"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J4" s="15" t="n">
         <v>12345678</v>
@@ -2591,117 +2724,117 @@
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L7" s="15" t="n">
         <v>8</v>
@@ -2712,34 +2845,34 @@
     </row>
     <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="n">
@@ -2751,31 +2884,31 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J9" s="12" t="n">
         <v>12345678</v>
@@ -2792,25 +2925,25 @@
       <c r="A10" s="11"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J10" s="20" t="n">
         <v>12345678</v>
@@ -2827,31 +2960,31 @@
       <c r="A11" s="11"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J11" s="20" t="n">
         <v>12345678</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L11" s="20" t="n">
         <v>8</v>
@@ -2864,31 +2997,31 @@
       <c r="A12" s="11"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L12" s="15" t="n">
         <v>32</v>
@@ -2899,57 +3032,57 @@
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E14" s="12" t="n">
         <v>1000</v>
@@ -2958,35 +3091,35 @@
         <v>-1</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="J14" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="20" t="n">
         <v>0</v>
@@ -2995,165 +3128,165 @@
         <v>0</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J16" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J18" s="20" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L19" s="15" t="n">
         <v>8</v>
@@ -3164,429 +3297,429 @@
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J22" s="20"/>
       <c r="K22" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J24" s="20" t="n">
         <v>10</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="17"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J25" s="20" t="n">
         <v>2</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J26" s="20"/>
       <c r="K26" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M26" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L27" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H29" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="I29" s="22" t="s">
-        <v>57</v>
       </c>
       <c r="J29" s="22" t="n">
         <v>1</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M30" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E31" s="12" t="n">
         <v>1000</v>
@@ -3595,33 +3728,33 @@
         <v>-1</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E32" s="20" t="n">
         <v>0</v>
@@ -3630,7 +3763,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
@@ -3643,19 +3776,19 @@
       <c r="A33" s="11"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -3666,16 +3799,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E34" s="12" t="n">
         <v>1000</v>
@@ -3684,19 +3817,19 @@
         <v>-1</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L34" s="12"/>
       <c r="M34" s="14"/>
@@ -3705,10 +3838,10 @@
       <c r="A35" s="11"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E35" s="20" t="n">
         <v>0</v>
@@ -3717,19 +3850,19 @@
         <v>0</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L35" s="20" t="n">
         <v>8</v>
@@ -3742,31 +3875,31 @@
       <c r="A36" s="11"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L36" s="20"/>
       <c r="M36" s="21"/>
@@ -3780,57 +3913,57 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L37" s="15"/>
       <c r="M37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H38" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I38" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="J38" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M38" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3842,13 +3975,13 @@
       <c r="F39" s="20"/>
       <c r="G39" s="20"/>
       <c r="H39" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
@@ -3863,13 +3996,13 @@
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
@@ -3877,41 +4010,41 @@
     </row>
     <row r="41" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H41" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I41" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="J41" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M41" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,20 +4056,20 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3969,7 +4102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3982,10 +4115,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="77.9838056680162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="94.9068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="80.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4001,90 +4134,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="93.2995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="79.6963562753036"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4106,18 +4173,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="60.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.4493927125506"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="63.6518218623482"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="79.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="80.9838056680162"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,16 +4199,50 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C3" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4158,29 +4259,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="70.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="90.8380566801619"/>
-    <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="62.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="63.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4189,32 +4289,10 @@
         <v>105</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4236,59 +4314,60 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="100.048582995951"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="81.4089068825911"/>
-    <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>112</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corporate user all senario done error in insert update
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="deactivateUserLogins" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="179">
   <si>
     <t>URL</t>
   </si>
@@ -571,7 +571,13 @@
     <t>/web-corporate/api/submit/corporate/user/insertUser</t>
   </si>
   <si>
+    <t>{"Header":{},"Params":{"UserName":"test82@gmail.com","Password":"12345678","FirstName":"test82","LastName":"test82","EmailAddress":"test82@gmail.com"}}</t>
+  </si>
+  <si>
     <t>jsonSchema/corporate/user/insertUser.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/user/insertUserParamError.json</t>
   </si>
   <si>
     <t>/web-corporate/api/submit/corporate/user/updateUser</t>
@@ -938,10 +944,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="107.226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="98.336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="85.3724696356275"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="109.153846153846"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="100.048582995951"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="86.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="85.3724696356275"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,8 +1029,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="105.51012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="85.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="107.441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="87.1943319838057"/>
     <col collapsed="false" hidden="false" max="1015" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1016" style="1" width="9.10526315789474"/>
   </cols>
@@ -1097,9 +1103,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="100.263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="143.753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="80.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="101.975708502024"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="146.323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="82.4817813765182"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1171,9 +1177,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="89.2307692307692"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="60.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="90.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="79.0526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1223,9 +1229,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.1295546558704"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.5182186234818"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -1275,9 +1281,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.2348178137652"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1327,9 +1333,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="60.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.663967611336"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1380,9 +1386,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1523,9 +1529,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="66.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="65.663967611336"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="67.5910931174089"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="55.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1597,10 +1603,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="67.8056680161943"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="55.165991902834"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="85.0526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="86.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="85.3724696356275"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,9 +1688,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="67.7004048582996"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="68.7692307692308"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="56.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1773,7 +1779,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1806,15 +1812,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="51.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1864,9 +1870,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="100.368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="102.085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1916,9 +1922,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.2307692307692"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="119.546558704453"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="90.8380566801619"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="121.793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1968,9 +1974,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="89.9797570850202"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.6923076923077"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2020,9 +2026,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="91.6923076923077"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2072,9 +2078,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="94.2631578947368"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="62.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2124,9 +2130,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="95.8704453441296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="97.587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="79.6963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="65.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2176,9 +2182,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="107.226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.5910931174089"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="109.153846153846"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="71.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2228,9 +2234,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="107.226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="120.935222672065"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.5910931174089"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="109.153846153846"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="123.080971659919"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="71.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2272,17 +2278,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="82.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="46.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="139.255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="87.6234817813765"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2301,44 +2307,22 @@
       <c r="A2" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>123</v>
+      <c r="B2" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="5" t="n">
-        <v>123</v>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2365,9 +2349,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="83.8744939271255"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="87.6234817813765"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2384,13 +2368,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2417,9 +2401,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="102.728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="104.546558704453"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2436,24 +2420,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2480,9 +2464,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="66.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="62.663967611336"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="67.5910931174089"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2499,13 +2483,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2532,9 +2516,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="107.226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="70.5910931174089"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="109.153846153846"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="71.7692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2586,19 +2570,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="7" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="7" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="7" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="7" width="14.1417004048583"/>
   </cols>
   <sheetData>
@@ -4129,10 +4113,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="80.6599190283401"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="98.336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="82.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="100.048582995951"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="85.3724696356275"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4195,10 +4179,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="65.7692307692308"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="83.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="85.3724696356275"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4281,9 +4265,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="64.8056680161943"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="64.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="65.8785425101215"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="65.2348178137652"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="66.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4333,9 +4317,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="95.7651821862348"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="97.4777327935223"/>
     <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="9.10526315789474"/>
   </cols>

</xml_diff>

<commit_message>
Refactoring Account Service, Adding Test Case Description in Log...
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" firstSheet="36" activeTab="44"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" firstSheet="31" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="API Request Matrix" sheetId="1" r:id="rId1"/>
@@ -39,19 +39,19 @@
     <sheet name="insertAccount" sheetId="30" r:id="rId30"/>
     <sheet name="updateAccounts" sheetId="31" r:id="rId31"/>
     <sheet name="updateAccount" sheetId="32" r:id="rId32"/>
-    <sheet name="getAccounts" sheetId="33" r:id="rId33"/>
-    <sheet name="readAccount" sheetId="34" r:id="rId34"/>
-    <sheet name="deleteAccount" sheetId="35" r:id="rId35"/>
-    <sheet name="getAccountContacts" sheetId="36" r:id="rId36"/>
-    <sheet name="getContacts" sheetId="37" r:id="rId37"/>
-    <sheet name="insertContacts" sheetId="38" r:id="rId38"/>
-    <sheet name="insertContact" sheetId="39" r:id="rId39"/>
-    <sheet name="updateContacts" sheetId="40" r:id="rId40"/>
-    <sheet name="updateContact" sheetId="41" r:id="rId41"/>
-    <sheet name="deleteContact" sheetId="42" r:id="rId42"/>
-    <sheet name="addAccountContactAffiliations" sheetId="43" r:id="rId43"/>
-    <sheet name="getCollection_reference" sheetId="44" r:id="rId44"/>
-    <sheet name="get_reference" sheetId="45" r:id="rId45"/>
+    <sheet name="deleteAccount" sheetId="35" r:id="rId33"/>
+    <sheet name="getAccountContacts" sheetId="36" r:id="rId34"/>
+    <sheet name="getContacts" sheetId="37" r:id="rId35"/>
+    <sheet name="insertContacts" sheetId="38" r:id="rId36"/>
+    <sheet name="insertContact" sheetId="39" r:id="rId37"/>
+    <sheet name="updateContacts" sheetId="40" r:id="rId38"/>
+    <sheet name="updateContact" sheetId="41" r:id="rId39"/>
+    <sheet name="deleteContact" sheetId="42" r:id="rId40"/>
+    <sheet name="addAccountContactAffiliations" sheetId="43" r:id="rId41"/>
+    <sheet name="getCollection_reference" sheetId="44" r:id="rId42"/>
+    <sheet name="get_reference" sheetId="45" r:id="rId43"/>
+    <sheet name="getCollection_account" sheetId="33" r:id="rId44"/>
+    <sheet name="get_account" sheetId="34" r:id="rId45"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="564">
   <si>
     <t>Api</t>
   </si>
@@ -737,129 +737,48 @@
     <t>jsonSchema/corporate/account/updateAccount_MaxLimitData.json</t>
   </si>
   <si>
-    <t>Test Case</t>
-  </si>
-  <si>
     <t>/web-corporate/api/submit/corporate/account/getAccounts</t>
   </si>
   <si>
-    <t>TC000</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"DESC"}]},"Params":{}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts.json</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{"AccountIDs":[1],"AccountName":"Test-AC002_UPD","AccountTypeIDs":[1001],"AccountTypeName":"Personal"}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_Filtered.json</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_PageSize.json</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":2,"StartPosition":1,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_StartPosition.json</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{"AccountIDs":[31,32]}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_AccountIDs.json</t>
-  </si>
-  <si>
-    <t>TC005</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{"AccountName":"Test-AC002_UPD"}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_AccountName.json</t>
-  </si>
-  <si>
-    <t>TC006</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{"AccountTypeIDs":[1,1001]}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_AccountTypeIDs.json</t>
-  </si>
-  <si>
-    <t>TC007</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{"AccountTypeName":"Individual"}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_AccountTypeName.json</t>
-  </si>
-  <si>
-    <t>TC008</t>
-  </si>
-  <si>
     <t>"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"ASC"}]},"Params":{"AccountTypeName":"Individual"}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/getAccounts_InvalidHTTPRequestBody.json</t>
-  </si>
-  <si>
-    <t>TC-001</t>
-  </si>
-  <si>
     <t>/web-corporate/api/submit/corporate/account/readAccount</t>
   </si>
   <si>
     <t>{"Header":{},"Params":{"AccountID":32}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/readAccount_AllParams.json</t>
-  </si>
-  <si>
-    <t>TC-002</t>
-  </si>
-  <si>
     <t>{"Header":{},"Params":{"AccountID":100}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/readAccount_non-existingAccountID.json</t>
-  </si>
-  <si>
-    <t>TC-003</t>
-  </si>
-  <si>
-    <t>jsonSchema/corporate/account/readAccount_WithoutAccountID.json</t>
-  </si>
-  <si>
-    <t>TC-004</t>
-  </si>
-  <si>
     <t>"Header":{},"Params":{"AccountID":32}}</t>
   </si>
   <si>
-    <t>jsonSchema/corporate/account/readAccount_InvalidHTTPRequestBody.json</t>
-  </si>
-  <si>
     <t>/web-corporate/api/submit/corporate/account/deleteAccount</t>
   </si>
   <si>
@@ -1193,9 +1112,6 @@
     <t>{"Header":{"ReferenceType":"AddressType"},"Params":{"Description":"Snail Mail Address"}}</t>
   </si>
   <si>
-    <t>{"Header":{"ReferenceType":"AddressType"},"Params":{"IDs":[2001]}}</t>
-  </si>
-  <si>
     <t>{"Header":{"ReferenceType":"RegionCode"},"Params":{}}</t>
   </si>
   <si>
@@ -1296,13 +1212,568 @@
   </si>
   <si>
     <t>jsonSchema/corporate/reference/get_reference_AccountType_failure.json</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AccountType_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AccountType_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AccountType_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AccountType_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AccountType_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AccountType_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_GenderType_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_GenderType_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_GenderType_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_GenderType_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_GenderType_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_GenderType_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AddressType_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AddressType_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AddressType_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AddressType_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AddressType_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AddressType_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_RegionCode_007</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_CountryCode_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_CountryCode_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_CountryCode_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_CountryCode_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_CountryCode_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_CountryCode_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AcAffiliationType_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AcAffiliationType_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AcAffiliationType_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AcAffiliationType_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AcAffiliationType_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_AcAffiliationType_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_PaymentType_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_PaymentType_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_PaymentType_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_PaymentType_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_PaymentType_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_PaymentType_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_REF_001</t>
+  </si>
+  <si>
+    <t>GET_REF_AccountType_001</t>
+  </si>
+  <si>
+    <t>GET_REF_AccountType_002</t>
+  </si>
+  <si>
+    <t>GET_REF_AccountType_003</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"GenderType"},"Params":{"ID":100}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"GenderType"},"Params":{"ID":1003}}</t>
+  </si>
+  <si>
+    <t>GET_REF_GenderType_001</t>
+  </si>
+  <si>
+    <t>GET_REF_GenderType_002</t>
+  </si>
+  <si>
+    <t>GET_REF_GenderType_003</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"AddressType"},"Params":{"IDs":[100]}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"AddressType"},"Params":{"ID":100}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"AddressType"},"Params":{"ID":2001}}</t>
+  </si>
+  <si>
+    <t>GET_REF_AddressType_001</t>
+  </si>
+  <si>
+    <t>GET_REF_AddressType_002</t>
+  </si>
+  <si>
+    <t>GET_REF_AddressType_003</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"RegionCode"},"Params":{"ID":2001}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"RegionCode"},"Params":{"ID":1}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"CountryCode"},"Params":{"ID":223}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"CountryCode"},"Params":{"ID":2001}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"AccountAffiliationType"},"Params":{"ID":2001}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"AccountAffiliationType"},"Params":{"ID":2}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"PaymentType"},"Params":{"ID":1}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"ReferenceType":"PaymentType"},"Params":{"ID":2001}}</t>
+  </si>
+  <si>
+    <t>GET_REF_RegionCode_001</t>
+  </si>
+  <si>
+    <t>GET_REF_RegionCode_002</t>
+  </si>
+  <si>
+    <t>GET_REF_RegionCode_003</t>
+  </si>
+  <si>
+    <t>GET_REF_CountryCode_001</t>
+  </si>
+  <si>
+    <t>GET_REF_CountryCode_002</t>
+  </si>
+  <si>
+    <t>GET_REF_CountryCode_003</t>
+  </si>
+  <si>
+    <t>GET_REF_AcAffiliationType_001</t>
+  </si>
+  <si>
+    <t>GET_REF_AcAffiliationType_002</t>
+  </si>
+  <si>
+    <t>GET_REF_AcAffiliationType_003</t>
+  </si>
+  <si>
+    <t>GET_REF_PaymentType_001</t>
+  </si>
+  <si>
+    <t>GET_REF_PaymentType_002</t>
+  </si>
+  <si>
+    <t>GET_REF_PaymentType_003</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_GenderType_success.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_GenderType_failure.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_AddressType_failure.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_CountryCode_failure.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_RegionCode_failure.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_AccountAffiliationType_failure.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_PaymentType_failure.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_AddressType_success.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_RegionCode_success.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_CountryCode_success.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_AccountAffiliationType_success.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/reference/get_reference_PaymentType_success.json</t>
+  </si>
+  <si>
+    <t>GET_REF_001</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"ID":4}}</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_001</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_002</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_005</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_006</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_007</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_008</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_009</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_Filtered.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_PageSize.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_StartPosition.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_AccountIDs.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_AccountName.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_AccountTypeIDs.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_AccountTypeName.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/getCollection_account_InvalidHTTPRequestBody.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/get_account_AllParams.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/get_account_non-existingAccountID.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/get_account_WithoutAccountID.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/account/get_account_InvalidHTTPRequestBody.json</t>
+  </si>
+  <si>
+    <t>GET_ACCOUNT_001</t>
+  </si>
+  <si>
+    <t>GET_ACCOUNT_002</t>
+  </si>
+  <si>
+    <t>GET_ACCOUNT_003</t>
+  </si>
+  <si>
+    <t>GET_ACCOUNT_004</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [Filtered List] when request params sent with ["IDs", "Name" &amp; "Description"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [Filtered List] when request params sent with ["IDs", "Name" &amp; "Description"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [Filtered List] when request params sent with ["IDs", "Name" &amp; "Description"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [Filtered List] when request params sent with ["IDs", "Name", "Description" &amp; "CountryCode"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [Filtered List] when request params sent with ["CountryCode"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [Filtered List] when request params sent with ["IDs", "Name" &amp; "Description"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountAffiliationType" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "AccountAffiliationType" api returns [Filtered List] when request params sent with ["IDs", "Name" &amp; "Description"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountAffiliationType" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountAffiliationType" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountAffiliationType" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountAffiliationType" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [Filtered List] when request params sent with ["IDs", "Name" &amp; "Description"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [Filtered List] when request params sent with ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [Filtered List] when request params sent with ["Description"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [NULL Data] when request params sent with non-existing ["IDs"]</t>
+  </si>
+  <si>
+    <t>Verify "Reference" api returns [error msg: "Reference type not found"] when request header sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "AccountType" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "GenderType" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "AddressType" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "RegionCode" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "CountryCode" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "AcAffiliationType" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "AcAffiliationType" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "AcAffiliationType" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns record when request params sent with existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [NULL Data] when request params sent with non-existing ["ID"]</t>
+  </si>
+  <si>
+    <t>Verify "PaymentType" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1355,6 +1826,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1491,7 +1969,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1587,6 +2065,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1595,12 +2086,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1991,7 +2476,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2030,7 +2515,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
         <v>17</v>
@@ -2225,7 +2710,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="42" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2264,7 +2749,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12" t="s">
         <v>17</v>
@@ -2299,7 +2784,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>17</v>
@@ -2336,7 +2821,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
         <v>17</v>
@@ -2414,7 +2899,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="42" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2455,7 +2940,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
         <v>45</v>
@@ -2492,7 +2977,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
         <v>48</v>
@@ -2529,7 +3014,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
         <v>17</v>
@@ -2564,7 +3049,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>17</v>
@@ -2601,7 +3086,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
         <v>17</v>
@@ -2679,7 +3164,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="42" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -2718,7 +3203,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
         <v>17</v>
@@ -2753,7 +3238,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>17</v>
@@ -2790,7 +3275,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="44" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -2829,7 +3314,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
         <v>17</v>
@@ -2864,7 +3349,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
         <v>17</v>
@@ -2899,7 +3384,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>17</v>
@@ -2934,7 +3419,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="7"/>
       <c r="C28" s="12" t="s">
         <v>17</v>
@@ -3051,7 +3536,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="42" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -3090,7 +3575,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12" t="s">
         <v>45</v>
@@ -3115,7 +3600,7 @@
       <c r="M32" s="13"/>
     </row>
     <row r="33" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>48</v>
@@ -3140,7 +3625,7 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="42" t="s">
         <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -3177,7 +3662,7 @@
       <c r="M34" s="6"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12" t="s">
         <v>45</v>
@@ -3214,7 +3699,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A36" s="37"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>48</v>
@@ -3247,7 +3732,7 @@
       <c r="M36" s="13"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -3270,7 +3755,7 @@
       <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -3309,7 +3794,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -3330,7 +3815,7 @@
       <c r="M39" s="13"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -3351,7 +3836,7 @@
       <c r="M40" s="13"/>
     </row>
     <row r="41" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="42" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -3390,7 +3875,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
+      <c r="A42" s="42"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -3416,11 +3901,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="A3:A4"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A42"/>
@@ -3429,6 +3909,11 @@
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1"/>
@@ -4996,266 +5481,6 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK10"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" activeCellId="1" sqref="C7 B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="59.140625" style="17"/>
-    <col min="2" max="2" width="25.7109375" style="17"/>
-    <col min="3" max="3" width="118.7109375" style="17"/>
-    <col min="4" max="4" width="63.5703125" style="17"/>
-    <col min="5" max="1025" width="8.140625" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>248</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" activeCellId="1" sqref="C7 B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13" style="17"/>
-    <col min="2" max="2" width="59.28515625" style="17"/>
-    <col min="3" max="3" width="52.28515625" style="17"/>
-    <col min="4" max="4" width="68.85546875" style="17"/>
-    <col min="5" max="1025" width="8.42578125" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>260</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK5"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -5283,46 +5508,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -5335,7 +5560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
@@ -5364,13 +5589,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5383,7 +5608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK6"/>
   <sheetViews>
@@ -6433,57 +6658,57 @@
     </row>
     <row r="2" spans="1:1024" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -6492,7 +6717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -6521,79 +6746,79 @@
     </row>
     <row r="2" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -6602,7 +6827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -6631,79 +6856,321 @@
     </row>
     <row r="2" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A7" activeCellId="1" sqref="C7 A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.85546875" style="32"/>
+    <col min="2" max="2" width="46.7109375" style="32"/>
+    <col min="3" max="3" width="75.7109375" style="32"/>
+    <col min="4" max="1025" width="8.7109375" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK9"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" activeCellId="1" sqref="C7 B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.85546875" style="32"/>
+    <col min="2" max="2" width="46.7109375" style="32"/>
+    <col min="3" max="3" width="61.7109375" style="32"/>
+    <col min="4" max="1025" width="8.7109375" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>293</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -6791,248 +7258,6 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK9"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" activeCellId="1" sqref="C7 A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="56.85546875" style="32"/>
-    <col min="2" max="2" width="46.7109375" style="32"/>
-    <col min="3" max="3" width="75.7109375" style="32"/>
-    <col min="4" max="1025" width="8.7109375" style="35"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="255" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>304</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>308</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>314</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK9"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" activeCellId="1" sqref="C7 B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="56.85546875" style="32"/>
-    <col min="2" max="2" width="46.7109375" style="32"/>
-    <col min="3" max="3" width="61.7109375" style="32"/>
-    <col min="4" max="1025" width="8.7109375" style="35"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>322</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>324</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>329</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>330</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK6"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -7061,57 +7286,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -7124,7 +7349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -7153,68 +7378,1275 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="111.140625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="63.28515625" customWidth="1"/>
+    <col min="4" max="4" width="140.5703125" style="32" customWidth="1"/>
+    <col min="5" max="5" width="93.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>501</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>502</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>503</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>499</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>505</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>387</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>507</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>389</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>508</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>509</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>510</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>392</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>393</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>512</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>394</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>513</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>395</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>396</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>515</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>397</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>516</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>517</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>399</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>400</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>347</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>401</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>520</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>402</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>521</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>403</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>522</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>404</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>523</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>346</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>405</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>524</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>406</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>525</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>407</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>526</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>408</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>527</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>409</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>528</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>529</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>411</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>412</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>531</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>413</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>532</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>414</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>415</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>534</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>416</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>535</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>417</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>418</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>537</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>419</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>538</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>420</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>539</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>421</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>422</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>541</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>423</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>542</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+    <col min="4" max="4" width="76" style="32" customWidth="1"/>
+    <col min="5" max="5" width="86" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>543</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>547</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>544</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>545</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>548</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>546</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>435</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>549</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>434</v>
+      </c>
+      <c r="E8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>433</v>
+      </c>
+      <c r="E9" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>437</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="E10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>552</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>439</v>
+      </c>
+      <c r="E11" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>447</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>553</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="E12" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>448</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>554</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="E13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>449</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>555</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>440</v>
+      </c>
+      <c r="E14" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>556</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="E15" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>451</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>557</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>452</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>558</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="E17" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>453</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>559</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>442</v>
+      </c>
+      <c r="E18" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>454</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>560</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="E19" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>455</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>561</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="E20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>456</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>562</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="E21" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>457</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>563</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="E22" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>470</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>542</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -7229,512 +8661,159 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:AMK10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.28515625" customWidth="1"/>
-    <col min="2" max="2" width="140.5703125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="93.85546875" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" style="17"/>
+    <col min="2" max="2" width="31.140625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="123.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="84.28515625" style="17" customWidth="1"/>
+    <col min="5" max="1025" width="8.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>353</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>472</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>350</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>357</v>
+        <v>221</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>474</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>351</v>
+        <v>223</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>475</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>352</v>
+        <v>224</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>476</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>354</v>
+        <v>225</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>477</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>358</v>
+        <v>226</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>478</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>361</v>
+        <v>227</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>479</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>362</v>
+        <v>228</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>480</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>364</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>366</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>369</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>373</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>379</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>375</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>380</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>374</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>381</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>384</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>382</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>386</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>387</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>388</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>391</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>392</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>393</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>394</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>397</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B44" s="32" t="s">
-        <v>398</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>355</v>
+        <v>229</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -7749,508 +8828,94 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:AMH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" customWidth="1"/>
-    <col min="2" max="2" width="140.5703125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="93.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19" style="17" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" style="17"/>
+    <col min="3" max="3" width="52.28515625" style="17"/>
+    <col min="4" max="4" width="68.85546875" style="17"/>
+    <col min="5" max="1022" width="8.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>403</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>494</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>404</v>
+        <v>231</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>353</v>
+        <v>232</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>362</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>364</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>366</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>369</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>373</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>379</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>375</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>380</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>374</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>381</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>384</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>382</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>386</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>387</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>388</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>391</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>392</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>393</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>394</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>397</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B44" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>398</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>355</v>
+        <v>86</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>493</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding GetCollection for Account...
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" firstSheet="31" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" firstSheet="31" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="API Request Matrix" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="581">
   <si>
     <t>Api</t>
   </si>
@@ -737,9 +737,6 @@
     <t>jsonSchema/corporate/account/updateAccount_MaxLimitData.json</t>
   </si>
   <si>
-    <t>/web-corporate/api/submit/corporate/account/getAccounts</t>
-  </si>
-  <si>
     <t>{"Header":{"PageSize":1000,"StartPosition":0,"Sort":[{"By":"ID","Dir":"DESC"}]},"Params":{}}</t>
   </si>
   <si>
@@ -1767,6 +1764,60 @@
   </si>
   <si>
     <t>Verify "PaymentType" api returns [error msg: "ID is required"] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/corporate/account/getCollection</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Complete List] when request params sent with [blank]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["AccountIDs", "Name", "AccountTypeIDs", "AccountTypeName", "PaymentTerm" &amp; "IsActive"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [List] acording to request header [PageSize] value</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [List] acording to request header [StartPosition] value</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [List] acording to request header [SortBy] value</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [List] acording to request header [SortDir] value</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["AccountIDs"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["Name"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["AccountTypeIDs"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["AccountTypeName"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["PaymentTerm"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [Filtered List] when request params sent with ["IsActive"]</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Account" returns [NULL Data] when request params sent with non-existing ["AccountIDs"]</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_010</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_011</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_012</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ACCOUNT_013</t>
   </si>
 </sst>
 </file>
@@ -2072,12 +2123,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2086,6 +2131,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2416,31 +2467,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2476,7 +2527,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2515,7 +2566,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
         <v>17</v>
@@ -2710,7 +2761,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2749,7 +2800,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12" t="s">
         <v>17</v>
@@ -2784,7 +2835,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
         <v>17</v>
@@ -2821,7 +2872,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
         <v>17</v>
@@ -2899,7 +2950,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2940,7 +2991,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
         <v>45</v>
@@ -2977,7 +3028,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
         <v>48</v>
@@ -3014,7 +3065,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
         <v>17</v>
@@ -3049,7 +3100,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
         <v>17</v>
@@ -3086,7 +3137,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
         <v>17</v>
@@ -3164,7 +3215,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="40" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -3203,7 +3254,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
         <v>17</v>
@@ -3238,7 +3289,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
         <v>17</v>
@@ -3275,7 +3326,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="42" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -3314,7 +3365,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
         <v>17</v>
@@ -3349,7 +3400,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
         <v>17</v>
@@ -3384,7 +3435,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
         <v>17</v>
@@ -3419,7 +3470,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="7"/>
       <c r="C28" s="12" t="s">
         <v>17</v>
@@ -3536,7 +3587,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="40" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -3575,7 +3626,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12" t="s">
         <v>45</v>
@@ -3600,7 +3651,7 @@
       <c r="M32" s="13"/>
     </row>
     <row r="33" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>48</v>
@@ -3625,7 +3676,7 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="40" t="s">
         <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -3662,7 +3713,7 @@
       <c r="M34" s="6"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12" t="s">
         <v>45</v>
@@ -3699,7 +3750,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="51" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>48</v>
@@ -3732,7 +3783,7 @@
       <c r="M36" s="13"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -3755,7 +3806,7 @@
       <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="41" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -3794,7 +3845,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -3815,7 +3866,7 @@
       <c r="M39" s="13"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -3836,7 +3887,7 @@
       <c r="M40" s="13"/>
     </row>
     <row r="41" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="40" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -3875,7 +3926,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -3901,6 +3952,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A3:A4"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A42"/>
@@ -3909,11 +3965,6 @@
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1"/>
@@ -5508,46 +5559,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>239</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -5589,13 +5640,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -6658,57 +6709,57 @@
     </row>
     <row r="2" spans="1:1024" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="C2" s="22" t="s">
         <v>245</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>247</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>249</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>251</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>253</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -6746,79 +6797,79 @@
     </row>
     <row r="2" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="C2" s="22" t="s">
         <v>256</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>258</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>256</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>262</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>264</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -6856,79 +6907,79 @@
     </row>
     <row r="2" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>268</v>
-      </c>
       <c r="C2" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>268</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -6966,90 +7017,90 @@
     </row>
     <row r="2" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>273</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>275</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>277</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>279</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>283</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>286</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -7087,90 +7138,90 @@
     </row>
     <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>289</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>291</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>293</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>295</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B6" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>297</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>299</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>302</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -7286,57 +7337,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>305</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>307</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>309</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>312</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -7378,68 +7429,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" t="s">
         <v>314</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="17" t="s">
         <v>315</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>318</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B7" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -7456,8 +7507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7471,10 +7522,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>80</v>
@@ -7488,750 +7539,750 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>323</v>
-      </c>
       <c r="E3" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D13" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>332</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D14" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>339</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D24" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>349</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D29" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>354</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D33" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>360</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D39" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>367</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -8249,7 +8300,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8263,10 +8314,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>80</v>
@@ -8280,373 +8331,373 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C2" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>375</v>
-      </c>
       <c r="E2" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D3" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>376</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E16" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E22" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>469</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>541</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>470</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>542</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>374</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -8661,160 +8712,279 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK10"/>
+  <dimension ref="A1:AML26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.140625" style="17"/>
-    <col min="2" max="2" width="31.140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="123.7109375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="84.28515625" style="17" customWidth="1"/>
-    <col min="5" max="1025" width="8.140625" style="17"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="127.140625" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="1026" width="8.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>379</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>564</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="E2" s="17" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>472</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="B3" s="32" t="s">
+        <v>565</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>473</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="B4" s="32" t="s">
+        <v>570</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>571</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>475</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>572</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>476</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>573</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>477</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>574</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>478</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>479</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>566</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E10" s="17" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>474</v>
-      </c>
-      <c r="C4" s="17" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>577</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>567</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E11" s="17" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>475</v>
-      </c>
-      <c r="C5" s="17" t="s">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>578</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>568</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E12" s="17" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>476</v>
-      </c>
-      <c r="C6" s="17" t="s">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>579</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>569</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E13" s="17" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>477</v>
-      </c>
-      <c r="C7" s="17" t="s">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>580</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>576</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>478</v>
-      </c>
-      <c r="C8" s="17" t="s">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
+      <c r="C15" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E15" s="17" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>479</v>
-      </c>
-      <c r="C9" s="17" t="s">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D16" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E16" s="17" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>489</v>
-      </c>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="32"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="32"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -8831,7 +9001,7 @@
   <dimension ref="A1:AMH5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B12:B13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8845,7 +9015,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>80</v>
@@ -8859,58 +9029,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>231</v>
-      </c>
       <c r="D2" s="17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding PostCollection for Address...
</commit_message>
<xml_diff>
--- a/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
+++ b/CorporateAPIAutomation/src/test/resources/config/Api_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" firstSheet="39" activeTab="47"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" firstSheet="40" activeTab="48"/>
   </bookViews>
   <sheets>
     <sheet name="API Request Matrix" sheetId="1" r:id="rId1"/>
@@ -55,6 +55,7 @@
     <sheet name="get_contact" sheetId="46" r:id="rId46"/>
     <sheet name="getCollection_address" sheetId="47" r:id="rId47"/>
     <sheet name="get_address" sheetId="48" r:id="rId48"/>
+    <sheet name="postCollection_address" sheetId="49" r:id="rId49"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="691">
   <si>
     <t>Api</t>
   </si>
@@ -2027,7 +2028,130 @@
     <t>Verify "getCollection" api for "Address" returns [List] according to request header [PageSize, StartPosition, SortBy, SortDir] value</t>
   </si>
   <si>
-    <t>Verify "getCollection" api for "Address" returns [NULL Data] when request params sent with non-existing ["ContactID" or "AccountID"]</t>
+    <t>{"Header":{"PageSize":3,"StartPosition":1,"SortBy":"ContactID","SortDir":"ASC"},"Params":{"ContactID":2}}</t>
+  </si>
+  <si>
+    <t>{"Header":{"PageSize":1000,"StartPosition":0,"SortBy":"ContactID","SortDir":"ASC"},"Params":{"ContactID":-1}}</t>
+  </si>
+  <si>
+    <t>Verify "getCollection" api for "Address" returns [Blank List] when request params sent with non-existing ["ContactID" or "AccountID"]</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/getCollection_address_Header.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/getCollection_address_non-existingParams.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/getCollection_address_WithoutParams.json</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ADDRESS_003</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ADDRESS_004</t>
+  </si>
+  <si>
+    <t>GETCOLLECTION_ADDRESS_005</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"ContactID":2,"AddressID": 41}}</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"AccountID":140,"AddressID": 50}}</t>
+  </si>
+  <si>
+    <t>Verify "get" api for "Address" returns record when request params sent with existing ["ContactID" &amp; "AddressID"]</t>
+  </si>
+  <si>
+    <t>Verify "get" api for "Address" returns record when request params sent with existing ["AccountID" &amp; "AddressID"]</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"AddressID": 50}}</t>
+  </si>
+  <si>
+    <t>Verify "get" api for "Address" returns [NULL Data] with "ERROR_MSG": "At least one param of [AccountID, ContactID] is required", when request params sent without ["ContactID" or "AccountID"]</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"AccountID":-140,"AddressID": -50}}</t>
+  </si>
+  <si>
+    <t>GET_ADDRESS_004</t>
+  </si>
+  <si>
+    <t>Verify "get" api for "Address" returns [NULL Data] with "ERROR_MSG": "Address not found for given params", when request params sent with non-existing ["AccountID"]</t>
+  </si>
+  <si>
+    <t>Verify "get" api for "Address" returns [NULL Data] with "ERROR_MSG": "Address not found for given params", when request params sent with non-existing ["ContactID"]</t>
+  </si>
+  <si>
+    <t>GET_ADDRESS_005</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"ContactID":-2,"AddressID": -41}}</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/get_address_non-existingParams.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/get_address_ContactID_AddressID.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/get_address_AccountID_AddressID.json</t>
+  </si>
+  <si>
+    <t>jsonSchema/corporate/address/get_address_WithoutRequiredParams.json</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_001</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_002</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_003</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_004</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_005</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_006</t>
+  </si>
+  <si>
+    <t>POSTCOLLECTION_ADDRESS_007</t>
+  </si>
+  <si>
+    <t>/web-corporate/api/submit/corporate/address/postCollection</t>
+  </si>
+  <si>
+    <t>Verify "postCollection" api for "address" creates record &amp; returns success response when request sent with required params [i.e."AddressTypeID", "ContactID" &amp; "AddressLine1"] with other optional params</t>
+  </si>
+  <si>
+    <t>Verify "postCollection" api for "address" creates record &amp; returns success response when request sent with required params [i.e."AddressTypeID", "AccountID" &amp; "AddressLine1"] with other optional params</t>
+  </si>
+  <si>
+    <t>Verify "postCollection" api for "address" creates record &amp; returns success response when request sent with only required params [i.e."AddressTypeID", "ContactID" &amp; "AddressLine1"]</t>
+  </si>
+  <si>
+    <t>Verify "postCollection" api for "address" creates record &amp; returns success response when request sent with only required params [i.e."AddressTypeID", "AccountID" &amp; "AddressLine1"]</t>
+  </si>
+  <si>
+    <t>Verify "postCollection" api for "address" doesn't create record &amp; returns [error msg: "Name is required"] when request sent without required param ["Name"]</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"Addresses":[{"AddressTypeID":21,"ContactID":25,"Locality":"acbd","RegionCodeID":11,"PostalCode":"1216","CountryCodeID":126,"IsConfidential":true,"IsPreferred":true,"AddressLine1":"sample","AddressLine2":"sample","AddressLine3":"sample"}]}}</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"Addresses":[{"AddressTypeID":21,"ContactID":28,"AddressLine1":"sample"}]}}</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"Addresses":[{"AddressTypeID":21,"AccountID":150,"Locality":"acbd","RegionCodeID":11,"PostalCode":"1216","CountryCodeID":126,"IsConfidential":true,"IsPreferred":true,"AddressLine1":"sample","AddressLine2":"sample","AddressLine3":"sample"}]}}</t>
+  </si>
+  <si>
+    <t>{"Header":{},"Params":{"Addresses":[{"AddressTypeID":21,"AccountID":151,"AddressLine1":"sample"}]}}</t>
   </si>
 </sst>
 </file>
@@ -7924,7 +8048,7 @@
   <dimension ref="A1:AMM8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8117,7 +8241,7 @@
   <dimension ref="A1:AMK8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8226,8 +8350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8347,8 +8471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" activeCellId="1" sqref="C7 B13"/>
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9745,7 +9869,7 @@
   <dimension ref="A1:AMM4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10867,25 +10991,25 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALP6"/>
+  <dimension ref="A1:ALJ6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="132.42578125" style="41" customWidth="1"/>
-    <col min="3" max="3" width="165.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.7109375" style="42" customWidth="1"/>
+    <col min="3" max="3" width="106.5703125" style="41" customWidth="1"/>
     <col min="4" max="4" width="61.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="80.85546875" style="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="1004" width="9.140625" style="29"/>
-    <col min="1005" max="16384" width="9.140625" style="41"/>
+    <col min="7" max="998" width="9.140625" style="29"/>
+    <col min="999" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:997" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>340</v>
       </c>
@@ -10893,6 +11017,1143 @@
         <v>446</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>576</v>
+      </c>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41"/>
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="41"/>
+      <c r="AS1" s="41"/>
+      <c r="AT1" s="41"/>
+      <c r="AU1" s="41"/>
+      <c r="AV1" s="41"/>
+      <c r="AW1" s="41"/>
+      <c r="AX1" s="41"/>
+      <c r="AY1" s="41"/>
+      <c r="AZ1" s="41"/>
+      <c r="BA1" s="41"/>
+      <c r="BB1" s="41"/>
+      <c r="BC1" s="41"/>
+      <c r="BD1" s="41"/>
+      <c r="BE1" s="41"/>
+      <c r="BF1" s="41"/>
+      <c r="BG1" s="41"/>
+      <c r="BH1" s="41"/>
+      <c r="BI1" s="41"/>
+      <c r="BJ1" s="41"/>
+      <c r="BK1" s="41"/>
+      <c r="BL1" s="41"/>
+      <c r="BM1" s="41"/>
+      <c r="BN1" s="41"/>
+      <c r="BO1" s="41"/>
+      <c r="BP1" s="41"/>
+      <c r="BQ1" s="41"/>
+      <c r="BR1" s="41"/>
+      <c r="BS1" s="41"/>
+      <c r="BT1" s="41"/>
+      <c r="BU1" s="41"/>
+      <c r="BV1" s="41"/>
+      <c r="BW1" s="41"/>
+      <c r="BX1" s="41"/>
+      <c r="BY1" s="41"/>
+      <c r="BZ1" s="41"/>
+      <c r="CA1" s="41"/>
+      <c r="CB1" s="41"/>
+      <c r="CC1" s="41"/>
+      <c r="CD1" s="41"/>
+      <c r="CE1" s="41"/>
+      <c r="CF1" s="41"/>
+      <c r="CG1" s="41"/>
+      <c r="CH1" s="41"/>
+      <c r="CI1" s="41"/>
+      <c r="CJ1" s="41"/>
+      <c r="CK1" s="41"/>
+      <c r="CL1" s="41"/>
+      <c r="CM1" s="41"/>
+      <c r="CN1" s="41"/>
+      <c r="CO1" s="41"/>
+      <c r="CP1" s="41"/>
+      <c r="CQ1" s="41"/>
+      <c r="CR1" s="41"/>
+      <c r="CS1" s="41"/>
+      <c r="CT1" s="41"/>
+      <c r="CU1" s="41"/>
+      <c r="CV1" s="41"/>
+      <c r="CW1" s="41"/>
+      <c r="CX1" s="41"/>
+      <c r="CY1" s="41"/>
+      <c r="CZ1" s="41"/>
+      <c r="DA1" s="41"/>
+      <c r="DB1" s="41"/>
+      <c r="DC1" s="41"/>
+      <c r="DD1" s="41"/>
+      <c r="DE1" s="41"/>
+      <c r="DF1" s="41"/>
+      <c r="DG1" s="41"/>
+      <c r="DH1" s="41"/>
+      <c r="DI1" s="41"/>
+      <c r="DJ1" s="41"/>
+      <c r="DK1" s="41"/>
+      <c r="DL1" s="41"/>
+      <c r="DM1" s="41"/>
+      <c r="DN1" s="41"/>
+      <c r="DO1" s="41"/>
+      <c r="DP1" s="41"/>
+      <c r="DQ1" s="41"/>
+      <c r="DR1" s="41"/>
+      <c r="DS1" s="41"/>
+      <c r="DT1" s="41"/>
+      <c r="DU1" s="41"/>
+      <c r="DV1" s="41"/>
+      <c r="DW1" s="41"/>
+      <c r="DX1" s="41"/>
+      <c r="DY1" s="41"/>
+      <c r="DZ1" s="41"/>
+      <c r="EA1" s="41"/>
+      <c r="EB1" s="41"/>
+      <c r="EC1" s="41"/>
+      <c r="ED1" s="41"/>
+      <c r="EE1" s="41"/>
+      <c r="EF1" s="41"/>
+      <c r="EG1" s="41"/>
+      <c r="EH1" s="41"/>
+      <c r="EI1" s="41"/>
+      <c r="EJ1" s="41"/>
+      <c r="EK1" s="41"/>
+      <c r="EL1" s="41"/>
+      <c r="EM1" s="41"/>
+      <c r="EN1" s="41"/>
+      <c r="EO1" s="41"/>
+      <c r="EP1" s="41"/>
+      <c r="EQ1" s="41"/>
+      <c r="ER1" s="41"/>
+      <c r="ES1" s="41"/>
+      <c r="ET1" s="41"/>
+      <c r="EU1" s="41"/>
+      <c r="EV1" s="41"/>
+      <c r="EW1" s="41"/>
+      <c r="EX1" s="41"/>
+      <c r="EY1" s="41"/>
+      <c r="EZ1" s="41"/>
+      <c r="FA1" s="41"/>
+      <c r="FB1" s="41"/>
+      <c r="FC1" s="41"/>
+      <c r="FD1" s="41"/>
+      <c r="FE1" s="41"/>
+      <c r="FF1" s="41"/>
+      <c r="FG1" s="41"/>
+      <c r="FH1" s="41"/>
+      <c r="FI1" s="41"/>
+      <c r="FJ1" s="41"/>
+      <c r="FK1" s="41"/>
+      <c r="FL1" s="41"/>
+      <c r="FM1" s="41"/>
+      <c r="FN1" s="41"/>
+      <c r="FO1" s="41"/>
+      <c r="FP1" s="41"/>
+      <c r="FQ1" s="41"/>
+      <c r="FR1" s="41"/>
+      <c r="FS1" s="41"/>
+      <c r="FT1" s="41"/>
+      <c r="FU1" s="41"/>
+      <c r="FV1" s="41"/>
+      <c r="FW1" s="41"/>
+      <c r="FX1" s="41"/>
+      <c r="FY1" s="41"/>
+      <c r="FZ1" s="41"/>
+      <c r="GA1" s="41"/>
+      <c r="GB1" s="41"/>
+      <c r="GC1" s="41"/>
+      <c r="GD1" s="41"/>
+      <c r="GE1" s="41"/>
+      <c r="GF1" s="41"/>
+      <c r="GG1" s="41"/>
+      <c r="GH1" s="41"/>
+      <c r="GI1" s="41"/>
+      <c r="GJ1" s="41"/>
+      <c r="GK1" s="41"/>
+      <c r="GL1" s="41"/>
+      <c r="GM1" s="41"/>
+      <c r="GN1" s="41"/>
+      <c r="GO1" s="41"/>
+      <c r="GP1" s="41"/>
+      <c r="GQ1" s="41"/>
+      <c r="GR1" s="41"/>
+      <c r="GS1" s="41"/>
+      <c r="GT1" s="41"/>
+      <c r="GU1" s="41"/>
+      <c r="GV1" s="41"/>
+      <c r="GW1" s="41"/>
+      <c r="GX1" s="41"/>
+      <c r="GY1" s="41"/>
+      <c r="GZ1" s="41"/>
+      <c r="HA1" s="41"/>
+      <c r="HB1" s="41"/>
+      <c r="HC1" s="41"/>
+      <c r="HD1" s="41"/>
+      <c r="HE1" s="41"/>
+      <c r="HF1" s="41"/>
+      <c r="HG1" s="41"/>
+      <c r="HH1" s="41"/>
+      <c r="HI1" s="41"/>
+      <c r="HJ1" s="41"/>
+      <c r="HK1" s="41"/>
+      <c r="HL1" s="41"/>
+      <c r="HM1" s="41"/>
+      <c r="HN1" s="41"/>
+      <c r="HO1" s="41"/>
+      <c r="HP1" s="41"/>
+      <c r="HQ1" s="41"/>
+      <c r="HR1" s="41"/>
+      <c r="HS1" s="41"/>
+      <c r="HT1" s="41"/>
+      <c r="HU1" s="41"/>
+      <c r="HV1" s="41"/>
+      <c r="HW1" s="41"/>
+      <c r="HX1" s="41"/>
+      <c r="HY1" s="41"/>
+      <c r="HZ1" s="41"/>
+      <c r="IA1" s="41"/>
+      <c r="IB1" s="41"/>
+      <c r="IC1" s="41"/>
+      <c r="ID1" s="41"/>
+      <c r="IE1" s="41"/>
+      <c r="IF1" s="41"/>
+      <c r="IG1" s="41"/>
+      <c r="IH1" s="41"/>
+      <c r="II1" s="41"/>
+      <c r="IJ1" s="41"/>
+      <c r="IK1" s="41"/>
+      <c r="IL1" s="41"/>
+      <c r="IM1" s="41"/>
+      <c r="IN1" s="41"/>
+      <c r="IO1" s="41"/>
+      <c r="IP1" s="41"/>
+      <c r="IQ1" s="41"/>
+      <c r="IR1" s="41"/>
+      <c r="IS1" s="41"/>
+      <c r="IT1" s="41"/>
+      <c r="IU1" s="41"/>
+      <c r="IV1" s="41"/>
+      <c r="IW1" s="41"/>
+      <c r="IX1" s="41"/>
+      <c r="IY1" s="41"/>
+      <c r="IZ1" s="41"/>
+      <c r="JA1" s="41"/>
+      <c r="JB1" s="41"/>
+      <c r="JC1" s="41"/>
+      <c r="JD1" s="41"/>
+      <c r="JE1" s="41"/>
+      <c r="JF1" s="41"/>
+      <c r="JG1" s="41"/>
+      <c r="JH1" s="41"/>
+      <c r="JI1" s="41"/>
+      <c r="JJ1" s="41"/>
+      <c r="JK1" s="41"/>
+      <c r="JL1" s="41"/>
+      <c r="JM1" s="41"/>
+      <c r="JN1" s="41"/>
+      <c r="JO1" s="41"/>
+      <c r="JP1" s="41"/>
+      <c r="JQ1" s="41"/>
+      <c r="JR1" s="41"/>
+      <c r="JS1" s="41"/>
+      <c r="JT1" s="41"/>
+      <c r="JU1" s="41"/>
+      <c r="JV1" s="41"/>
+      <c r="JW1" s="41"/>
+      <c r="JX1" s="41"/>
+      <c r="JY1" s="41"/>
+      <c r="JZ1" s="41"/>
+      <c r="KA1" s="41"/>
+      <c r="KB1" s="41"/>
+      <c r="KC1" s="41"/>
+      <c r="KD1" s="41"/>
+      <c r="KE1" s="41"/>
+      <c r="KF1" s="41"/>
+      <c r="KG1" s="41"/>
+      <c r="KH1" s="41"/>
+      <c r="KI1" s="41"/>
+      <c r="KJ1" s="41"/>
+      <c r="KK1" s="41"/>
+      <c r="KL1" s="41"/>
+      <c r="KM1" s="41"/>
+      <c r="KN1" s="41"/>
+      <c r="KO1" s="41"/>
+      <c r="KP1" s="41"/>
+      <c r="KQ1" s="41"/>
+      <c r="KR1" s="41"/>
+      <c r="KS1" s="41"/>
+      <c r="KT1" s="41"/>
+      <c r="KU1" s="41"/>
+      <c r="KV1" s="41"/>
+      <c r="KW1" s="41"/>
+      <c r="KX1" s="41"/>
+      <c r="KY1" s="41"/>
+      <c r="KZ1" s="41"/>
+      <c r="LA1" s="41"/>
+      <c r="LB1" s="41"/>
+      <c r="LC1" s="41"/>
+      <c r="LD1" s="41"/>
+      <c r="LE1" s="41"/>
+      <c r="LF1" s="41"/>
+      <c r="LG1" s="41"/>
+      <c r="LH1" s="41"/>
+      <c r="LI1" s="41"/>
+      <c r="LJ1" s="41"/>
+      <c r="LK1" s="41"/>
+      <c r="LL1" s="41"/>
+      <c r="LM1" s="41"/>
+      <c r="LN1" s="41"/>
+      <c r="LO1" s="41"/>
+      <c r="LP1" s="41"/>
+      <c r="LQ1" s="41"/>
+      <c r="LR1" s="41"/>
+      <c r="LS1" s="41"/>
+      <c r="LT1" s="41"/>
+      <c r="LU1" s="41"/>
+      <c r="LV1" s="41"/>
+      <c r="LW1" s="41"/>
+      <c r="LX1" s="41"/>
+      <c r="LY1" s="41"/>
+      <c r="LZ1" s="41"/>
+      <c r="MA1" s="41"/>
+      <c r="MB1" s="41"/>
+      <c r="MC1" s="41"/>
+      <c r="MD1" s="41"/>
+      <c r="ME1" s="41"/>
+      <c r="MF1" s="41"/>
+      <c r="MG1" s="41"/>
+      <c r="MH1" s="41"/>
+      <c r="MI1" s="41"/>
+      <c r="MJ1" s="41"/>
+      <c r="MK1" s="41"/>
+      <c r="ML1" s="41"/>
+      <c r="MM1" s="41"/>
+      <c r="MN1" s="41"/>
+      <c r="MO1" s="41"/>
+      <c r="MP1" s="41"/>
+      <c r="MQ1" s="41"/>
+      <c r="MR1" s="41"/>
+      <c r="MS1" s="41"/>
+      <c r="MT1" s="41"/>
+      <c r="MU1" s="41"/>
+      <c r="MV1" s="41"/>
+      <c r="MW1" s="41"/>
+      <c r="MX1" s="41"/>
+      <c r="MY1" s="41"/>
+      <c r="MZ1" s="41"/>
+      <c r="NA1" s="41"/>
+      <c r="NB1" s="41"/>
+      <c r="NC1" s="41"/>
+      <c r="ND1" s="41"/>
+      <c r="NE1" s="41"/>
+      <c r="NF1" s="41"/>
+      <c r="NG1" s="41"/>
+      <c r="NH1" s="41"/>
+      <c r="NI1" s="41"/>
+      <c r="NJ1" s="41"/>
+      <c r="NK1" s="41"/>
+      <c r="NL1" s="41"/>
+      <c r="NM1" s="41"/>
+      <c r="NN1" s="41"/>
+      <c r="NO1" s="41"/>
+      <c r="NP1" s="41"/>
+      <c r="NQ1" s="41"/>
+      <c r="NR1" s="41"/>
+      <c r="NS1" s="41"/>
+      <c r="NT1" s="41"/>
+      <c r="NU1" s="41"/>
+      <c r="NV1" s="41"/>
+      <c r="NW1" s="41"/>
+      <c r="NX1" s="41"/>
+      <c r="NY1" s="41"/>
+      <c r="NZ1" s="41"/>
+      <c r="OA1" s="41"/>
+      <c r="OB1" s="41"/>
+      <c r="OC1" s="41"/>
+      <c r="OD1" s="41"/>
+      <c r="OE1" s="41"/>
+      <c r="OF1" s="41"/>
+      <c r="OG1" s="41"/>
+      <c r="OH1" s="41"/>
+      <c r="OI1" s="41"/>
+      <c r="OJ1" s="41"/>
+      <c r="OK1" s="41"/>
+      <c r="OL1" s="41"/>
+      <c r="OM1" s="41"/>
+      <c r="ON1" s="41"/>
+      <c r="OO1" s="41"/>
+      <c r="OP1" s="41"/>
+      <c r="OQ1" s="41"/>
+      <c r="OR1" s="41"/>
+      <c r="OS1" s="41"/>
+      <c r="OT1" s="41"/>
+      <c r="OU1" s="41"/>
+      <c r="OV1" s="41"/>
+      <c r="OW1" s="41"/>
+      <c r="OX1" s="41"/>
+      <c r="OY1" s="41"/>
+      <c r="OZ1" s="41"/>
+      <c r="PA1" s="41"/>
+      <c r="PB1" s="41"/>
+      <c r="PC1" s="41"/>
+      <c r="PD1" s="41"/>
+      <c r="PE1" s="41"/>
+      <c r="PF1" s="41"/>
+      <c r="PG1" s="41"/>
+      <c r="PH1" s="41"/>
+      <c r="PI1" s="41"/>
+      <c r="PJ1" s="41"/>
+      <c r="PK1" s="41"/>
+      <c r="PL1" s="41"/>
+      <c r="PM1" s="41"/>
+      <c r="PN1" s="41"/>
+      <c r="PO1" s="41"/>
+      <c r="PP1" s="41"/>
+      <c r="PQ1" s="41"/>
+      <c r="PR1" s="41"/>
+      <c r="PS1" s="41"/>
+      <c r="PT1" s="41"/>
+      <c r="PU1" s="41"/>
+      <c r="PV1" s="41"/>
+      <c r="PW1" s="41"/>
+      <c r="PX1" s="41"/>
+      <c r="PY1" s="41"/>
+      <c r="PZ1" s="41"/>
+      <c r="QA1" s="41"/>
+      <c r="QB1" s="41"/>
+      <c r="QC1" s="41"/>
+      <c r="QD1" s="41"/>
+      <c r="QE1" s="41"/>
+      <c r="QF1" s="41"/>
+      <c r="QG1" s="41"/>
+      <c r="QH1" s="41"/>
+      <c r="QI1" s="41"/>
+      <c r="QJ1" s="41"/>
+      <c r="QK1" s="41"/>
+      <c r="QL1" s="41"/>
+      <c r="QM1" s="41"/>
+      <c r="QN1" s="41"/>
+      <c r="QO1" s="41"/>
+      <c r="QP1" s="41"/>
+      <c r="QQ1" s="41"/>
+      <c r="QR1" s="41"/>
+      <c r="QS1" s="41"/>
+      <c r="QT1" s="41"/>
+      <c r="QU1" s="41"/>
+      <c r="QV1" s="41"/>
+      <c r="QW1" s="41"/>
+      <c r="QX1" s="41"/>
+      <c r="QY1" s="41"/>
+      <c r="QZ1" s="41"/>
+      <c r="RA1" s="41"/>
+      <c r="RB1" s="41"/>
+      <c r="RC1" s="41"/>
+      <c r="RD1" s="41"/>
+      <c r="RE1" s="41"/>
+      <c r="RF1" s="41"/>
+      <c r="RG1" s="41"/>
+      <c r="RH1" s="41"/>
+      <c r="RI1" s="41"/>
+      <c r="RJ1" s="41"/>
+      <c r="RK1" s="41"/>
+      <c r="RL1" s="41"/>
+      <c r="RM1" s="41"/>
+      <c r="RN1" s="41"/>
+      <c r="RO1" s="41"/>
+      <c r="RP1" s="41"/>
+      <c r="RQ1" s="41"/>
+      <c r="RR1" s="41"/>
+      <c r="RS1" s="41"/>
+      <c r="RT1" s="41"/>
+      <c r="RU1" s="41"/>
+      <c r="RV1" s="41"/>
+      <c r="RW1" s="41"/>
+      <c r="RX1" s="41"/>
+      <c r="RY1" s="41"/>
+      <c r="RZ1" s="41"/>
+      <c r="SA1" s="41"/>
+      <c r="SB1" s="41"/>
+      <c r="SC1" s="41"/>
+      <c r="SD1" s="41"/>
+      <c r="SE1" s="41"/>
+      <c r="SF1" s="41"/>
+      <c r="SG1" s="41"/>
+      <c r="SH1" s="41"/>
+      <c r="SI1" s="41"/>
+      <c r="SJ1" s="41"/>
+      <c r="SK1" s="41"/>
+      <c r="SL1" s="41"/>
+      <c r="SM1" s="41"/>
+      <c r="SN1" s="41"/>
+      <c r="SO1" s="41"/>
+      <c r="SP1" s="41"/>
+      <c r="SQ1" s="41"/>
+      <c r="SR1" s="41"/>
+      <c r="SS1" s="41"/>
+      <c r="ST1" s="41"/>
+      <c r="SU1" s="41"/>
+      <c r="SV1" s="41"/>
+      <c r="SW1" s="41"/>
+      <c r="SX1" s="41"/>
+      <c r="SY1" s="41"/>
+      <c r="SZ1" s="41"/>
+      <c r="TA1" s="41"/>
+      <c r="TB1" s="41"/>
+      <c r="TC1" s="41"/>
+      <c r="TD1" s="41"/>
+      <c r="TE1" s="41"/>
+      <c r="TF1" s="41"/>
+      <c r="TG1" s="41"/>
+      <c r="TH1" s="41"/>
+      <c r="TI1" s="41"/>
+      <c r="TJ1" s="41"/>
+      <c r="TK1" s="41"/>
+      <c r="TL1" s="41"/>
+      <c r="TM1" s="41"/>
+      <c r="TN1" s="41"/>
+      <c r="TO1" s="41"/>
+      <c r="TP1" s="41"/>
+      <c r="TQ1" s="41"/>
+      <c r="TR1" s="41"/>
+      <c r="TS1" s="41"/>
+      <c r="TT1" s="41"/>
+      <c r="TU1" s="41"/>
+      <c r="TV1" s="41"/>
+      <c r="TW1" s="41"/>
+      <c r="TX1" s="41"/>
+      <c r="TY1" s="41"/>
+      <c r="TZ1" s="41"/>
+      <c r="UA1" s="41"/>
+      <c r="UB1" s="41"/>
+      <c r="UC1" s="41"/>
+      <c r="UD1" s="41"/>
+      <c r="UE1" s="41"/>
+      <c r="UF1" s="41"/>
+      <c r="UG1" s="41"/>
+      <c r="UH1" s="41"/>
+      <c r="UI1" s="41"/>
+      <c r="UJ1" s="41"/>
+      <c r="UK1" s="41"/>
+      <c r="UL1" s="41"/>
+      <c r="UM1" s="41"/>
+      <c r="UN1" s="41"/>
+      <c r="UO1" s="41"/>
+      <c r="UP1" s="41"/>
+      <c r="UQ1" s="41"/>
+      <c r="UR1" s="41"/>
+      <c r="US1" s="41"/>
+      <c r="UT1" s="41"/>
+      <c r="UU1" s="41"/>
+      <c r="UV1" s="41"/>
+      <c r="UW1" s="41"/>
+      <c r="UX1" s="41"/>
+      <c r="UY1" s="41"/>
+      <c r="UZ1" s="41"/>
+      <c r="VA1" s="41"/>
+      <c r="VB1" s="41"/>
+      <c r="VC1" s="41"/>
+      <c r="VD1" s="41"/>
+      <c r="VE1" s="41"/>
+      <c r="VF1" s="41"/>
+      <c r="VG1" s="41"/>
+      <c r="VH1" s="41"/>
+      <c r="VI1" s="41"/>
+      <c r="VJ1" s="41"/>
+      <c r="VK1" s="41"/>
+      <c r="VL1" s="41"/>
+      <c r="VM1" s="41"/>
+      <c r="VN1" s="41"/>
+      <c r="VO1" s="41"/>
+      <c r="VP1" s="41"/>
+      <c r="VQ1" s="41"/>
+      <c r="VR1" s="41"/>
+      <c r="VS1" s="41"/>
+      <c r="VT1" s="41"/>
+      <c r="VU1" s="41"/>
+      <c r="VV1" s="41"/>
+      <c r="VW1" s="41"/>
+      <c r="VX1" s="41"/>
+      <c r="VY1" s="41"/>
+      <c r="VZ1" s="41"/>
+      <c r="WA1" s="41"/>
+      <c r="WB1" s="41"/>
+      <c r="WC1" s="41"/>
+      <c r="WD1" s="41"/>
+      <c r="WE1" s="41"/>
+      <c r="WF1" s="41"/>
+      <c r="WG1" s="41"/>
+      <c r="WH1" s="41"/>
+      <c r="WI1" s="41"/>
+      <c r="WJ1" s="41"/>
+      <c r="WK1" s="41"/>
+      <c r="WL1" s="41"/>
+      <c r="WM1" s="41"/>
+      <c r="WN1" s="41"/>
+      <c r="WO1" s="41"/>
+      <c r="WP1" s="41"/>
+      <c r="WQ1" s="41"/>
+      <c r="WR1" s="41"/>
+      <c r="WS1" s="41"/>
+      <c r="WT1" s="41"/>
+      <c r="WU1" s="41"/>
+      <c r="WV1" s="41"/>
+      <c r="WW1" s="41"/>
+      <c r="WX1" s="41"/>
+      <c r="WY1" s="41"/>
+      <c r="WZ1" s="41"/>
+      <c r="XA1" s="41"/>
+      <c r="XB1" s="41"/>
+      <c r="XC1" s="41"/>
+      <c r="XD1" s="41"/>
+      <c r="XE1" s="41"/>
+      <c r="XF1" s="41"/>
+      <c r="XG1" s="41"/>
+      <c r="XH1" s="41"/>
+      <c r="XI1" s="41"/>
+      <c r="XJ1" s="41"/>
+      <c r="XK1" s="41"/>
+      <c r="XL1" s="41"/>
+      <c r="XM1" s="41"/>
+      <c r="XN1" s="41"/>
+      <c r="XO1" s="41"/>
+      <c r="XP1" s="41"/>
+      <c r="XQ1" s="41"/>
+      <c r="XR1" s="41"/>
+      <c r="XS1" s="41"/>
+      <c r="XT1" s="41"/>
+      <c r="XU1" s="41"/>
+      <c r="XV1" s="41"/>
+      <c r="XW1" s="41"/>
+      <c r="XX1" s="41"/>
+      <c r="XY1" s="41"/>
+      <c r="XZ1" s="41"/>
+      <c r="YA1" s="41"/>
+      <c r="YB1" s="41"/>
+      <c r="YC1" s="41"/>
+      <c r="YD1" s="41"/>
+      <c r="YE1" s="41"/>
+      <c r="YF1" s="41"/>
+      <c r="YG1" s="41"/>
+      <c r="YH1" s="41"/>
+      <c r="YI1" s="41"/>
+      <c r="YJ1" s="41"/>
+      <c r="YK1" s="41"/>
+      <c r="YL1" s="41"/>
+      <c r="YM1" s="41"/>
+      <c r="YN1" s="41"/>
+      <c r="YO1" s="41"/>
+      <c r="YP1" s="41"/>
+      <c r="YQ1" s="41"/>
+      <c r="YR1" s="41"/>
+      <c r="YS1" s="41"/>
+      <c r="YT1" s="41"/>
+      <c r="YU1" s="41"/>
+      <c r="YV1" s="41"/>
+      <c r="YW1" s="41"/>
+      <c r="YX1" s="41"/>
+      <c r="YY1" s="41"/>
+      <c r="YZ1" s="41"/>
+      <c r="ZA1" s="41"/>
+      <c r="ZB1" s="41"/>
+      <c r="ZC1" s="41"/>
+      <c r="ZD1" s="41"/>
+      <c r="ZE1" s="41"/>
+      <c r="ZF1" s="41"/>
+      <c r="ZG1" s="41"/>
+      <c r="ZH1" s="41"/>
+      <c r="ZI1" s="41"/>
+      <c r="ZJ1" s="41"/>
+      <c r="ZK1" s="41"/>
+      <c r="ZL1" s="41"/>
+      <c r="ZM1" s="41"/>
+      <c r="ZN1" s="41"/>
+      <c r="ZO1" s="41"/>
+      <c r="ZP1" s="41"/>
+      <c r="ZQ1" s="41"/>
+      <c r="ZR1" s="41"/>
+      <c r="ZS1" s="41"/>
+      <c r="ZT1" s="41"/>
+      <c r="ZU1" s="41"/>
+      <c r="ZV1" s="41"/>
+      <c r="ZW1" s="41"/>
+      <c r="ZX1" s="41"/>
+      <c r="ZY1" s="41"/>
+      <c r="ZZ1" s="41"/>
+      <c r="AAA1" s="41"/>
+      <c r="AAB1" s="41"/>
+      <c r="AAC1" s="41"/>
+      <c r="AAD1" s="41"/>
+      <c r="AAE1" s="41"/>
+      <c r="AAF1" s="41"/>
+      <c r="AAG1" s="41"/>
+      <c r="AAH1" s="41"/>
+      <c r="AAI1" s="41"/>
+      <c r="AAJ1" s="41"/>
+      <c r="AAK1" s="41"/>
+      <c r="AAL1" s="41"/>
+      <c r="AAM1" s="41"/>
+      <c r="AAN1" s="41"/>
+      <c r="AAO1" s="41"/>
+      <c r="AAP1" s="41"/>
+      <c r="AAQ1" s="41"/>
+      <c r="AAR1" s="41"/>
+      <c r="AAS1" s="41"/>
+      <c r="AAT1" s="41"/>
+      <c r="AAU1" s="41"/>
+      <c r="AAV1" s="41"/>
+      <c r="AAW1" s="41"/>
+      <c r="AAX1" s="41"/>
+      <c r="AAY1" s="41"/>
+      <c r="AAZ1" s="41"/>
+      <c r="ABA1" s="41"/>
+      <c r="ABB1" s="41"/>
+      <c r="ABC1" s="41"/>
+      <c r="ABD1" s="41"/>
+      <c r="ABE1" s="41"/>
+      <c r="ABF1" s="41"/>
+      <c r="ABG1" s="41"/>
+      <c r="ABH1" s="41"/>
+      <c r="ABI1" s="41"/>
+      <c r="ABJ1" s="41"/>
+      <c r="ABK1" s="41"/>
+      <c r="ABL1" s="41"/>
+      <c r="ABM1" s="41"/>
+      <c r="ABN1" s="41"/>
+      <c r="ABO1" s="41"/>
+      <c r="ABP1" s="41"/>
+      <c r="ABQ1" s="41"/>
+      <c r="ABR1" s="41"/>
+      <c r="ABS1" s="41"/>
+      <c r="ABT1" s="41"/>
+      <c r="ABU1" s="41"/>
+      <c r="ABV1" s="41"/>
+      <c r="ABW1" s="41"/>
+      <c r="ABX1" s="41"/>
+      <c r="ABY1" s="41"/>
+      <c r="ABZ1" s="41"/>
+      <c r="ACA1" s="41"/>
+      <c r="ACB1" s="41"/>
+      <c r="ACC1" s="41"/>
+      <c r="ACD1" s="41"/>
+      <c r="ACE1" s="41"/>
+      <c r="ACF1" s="41"/>
+      <c r="ACG1" s="41"/>
+      <c r="ACH1" s="41"/>
+      <c r="ACI1" s="41"/>
+      <c r="ACJ1" s="41"/>
+      <c r="ACK1" s="41"/>
+      <c r="ACL1" s="41"/>
+      <c r="ACM1" s="41"/>
+      <c r="ACN1" s="41"/>
+      <c r="ACO1" s="41"/>
+      <c r="ACP1" s="41"/>
+      <c r="ACQ1" s="41"/>
+      <c r="ACR1" s="41"/>
+      <c r="ACS1" s="41"/>
+      <c r="ACT1" s="41"/>
+      <c r="ACU1" s="41"/>
+      <c r="ACV1" s="41"/>
+      <c r="ACW1" s="41"/>
+      <c r="ACX1" s="41"/>
+      <c r="ACY1" s="41"/>
+      <c r="ACZ1" s="41"/>
+      <c r="ADA1" s="41"/>
+      <c r="ADB1" s="41"/>
+      <c r="ADC1" s="41"/>
+      <c r="ADD1" s="41"/>
+      <c r="ADE1" s="41"/>
+      <c r="ADF1" s="41"/>
+      <c r="ADG1" s="41"/>
+      <c r="ADH1" s="41"/>
+      <c r="ADI1" s="41"/>
+      <c r="ADJ1" s="41"/>
+      <c r="ADK1" s="41"/>
+      <c r="ADL1" s="41"/>
+      <c r="ADM1" s="41"/>
+      <c r="ADN1" s="41"/>
+      <c r="ADO1" s="41"/>
+      <c r="ADP1" s="41"/>
+      <c r="ADQ1" s="41"/>
+      <c r="ADR1" s="41"/>
+      <c r="ADS1" s="41"/>
+      <c r="ADT1" s="41"/>
+      <c r="ADU1" s="41"/>
+      <c r="ADV1" s="41"/>
+      <c r="ADW1" s="41"/>
+      <c r="ADX1" s="41"/>
+      <c r="ADY1" s="41"/>
+      <c r="ADZ1" s="41"/>
+      <c r="AEA1" s="41"/>
+      <c r="AEB1" s="41"/>
+      <c r="AEC1" s="41"/>
+      <c r="AED1" s="41"/>
+      <c r="AEE1" s="41"/>
+      <c r="AEF1" s="41"/>
+      <c r="AEG1" s="41"/>
+      <c r="AEH1" s="41"/>
+      <c r="AEI1" s="41"/>
+      <c r="AEJ1" s="41"/>
+      <c r="AEK1" s="41"/>
+      <c r="AEL1" s="41"/>
+      <c r="AEM1" s="41"/>
+      <c r="AEN1" s="41"/>
+      <c r="AEO1" s="41"/>
+      <c r="AEP1" s="41"/>
+      <c r="AEQ1" s="41"/>
+      <c r="AER1" s="41"/>
+      <c r="AES1" s="41"/>
+      <c r="AET1" s="41"/>
+      <c r="AEU1" s="41"/>
+      <c r="AEV1" s="41"/>
+      <c r="AEW1" s="41"/>
+      <c r="AEX1" s="41"/>
+      <c r="AEY1" s="41"/>
+      <c r="AEZ1" s="41"/>
+      <c r="AFA1" s="41"/>
+      <c r="AFB1" s="41"/>
+      <c r="AFC1" s="41"/>
+      <c r="AFD1" s="41"/>
+      <c r="AFE1" s="41"/>
+      <c r="AFF1" s="41"/>
+      <c r="AFG1" s="41"/>
+      <c r="AFH1" s="41"/>
+      <c r="AFI1" s="41"/>
+      <c r="AFJ1" s="41"/>
+      <c r="AFK1" s="41"/>
+      <c r="AFL1" s="41"/>
+      <c r="AFM1" s="41"/>
+      <c r="AFN1" s="41"/>
+      <c r="AFO1" s="41"/>
+      <c r="AFP1" s="41"/>
+      <c r="AFQ1" s="41"/>
+      <c r="AFR1" s="41"/>
+      <c r="AFS1" s="41"/>
+      <c r="AFT1" s="41"/>
+      <c r="AFU1" s="41"/>
+      <c r="AFV1" s="41"/>
+      <c r="AFW1" s="41"/>
+      <c r="AFX1" s="41"/>
+      <c r="AFY1" s="41"/>
+      <c r="AFZ1" s="41"/>
+      <c r="AGA1" s="41"/>
+      <c r="AGB1" s="41"/>
+      <c r="AGC1" s="41"/>
+      <c r="AGD1" s="41"/>
+      <c r="AGE1" s="41"/>
+      <c r="AGF1" s="41"/>
+      <c r="AGG1" s="41"/>
+      <c r="AGH1" s="41"/>
+      <c r="AGI1" s="41"/>
+      <c r="AGJ1" s="41"/>
+      <c r="AGK1" s="41"/>
+      <c r="AGL1" s="41"/>
+      <c r="AGM1" s="41"/>
+      <c r="AGN1" s="41"/>
+      <c r="AGO1" s="41"/>
+      <c r="AGP1" s="41"/>
+      <c r="AGQ1" s="41"/>
+      <c r="AGR1" s="41"/>
+      <c r="AGS1" s="41"/>
+      <c r="AGT1" s="41"/>
+      <c r="AGU1" s="41"/>
+      <c r="AGV1" s="41"/>
+      <c r="AGW1" s="41"/>
+      <c r="AGX1" s="41"/>
+      <c r="AGY1" s="41"/>
+      <c r="AGZ1" s="41"/>
+      <c r="AHA1" s="41"/>
+      <c r="AHB1" s="41"/>
+      <c r="AHC1" s="41"/>
+      <c r="AHD1" s="41"/>
+      <c r="AHE1" s="41"/>
+      <c r="AHF1" s="41"/>
+      <c r="AHG1" s="41"/>
+      <c r="AHH1" s="41"/>
+      <c r="AHI1" s="41"/>
+      <c r="AHJ1" s="41"/>
+      <c r="AHK1" s="41"/>
+      <c r="AHL1" s="41"/>
+      <c r="AHM1" s="41"/>
+      <c r="AHN1" s="41"/>
+      <c r="AHO1" s="41"/>
+      <c r="AHP1" s="41"/>
+      <c r="AHQ1" s="41"/>
+      <c r="AHR1" s="41"/>
+      <c r="AHS1" s="41"/>
+      <c r="AHT1" s="41"/>
+      <c r="AHU1" s="41"/>
+      <c r="AHV1" s="41"/>
+      <c r="AHW1" s="41"/>
+      <c r="AHX1" s="41"/>
+      <c r="AHY1" s="41"/>
+      <c r="AHZ1" s="41"/>
+      <c r="AIA1" s="41"/>
+      <c r="AIB1" s="41"/>
+      <c r="AIC1" s="41"/>
+      <c r="AID1" s="41"/>
+      <c r="AIE1" s="41"/>
+      <c r="AIF1" s="41"/>
+      <c r="AIG1" s="41"/>
+      <c r="AIH1" s="41"/>
+      <c r="AII1" s="41"/>
+      <c r="AIJ1" s="41"/>
+      <c r="AIK1" s="41"/>
+      <c r="AIL1" s="41"/>
+      <c r="AIM1" s="41"/>
+      <c r="AIN1" s="41"/>
+      <c r="AIO1" s="41"/>
+      <c r="AIP1" s="41"/>
+      <c r="AIQ1" s="41"/>
+      <c r="AIR1" s="41"/>
+      <c r="AIS1" s="41"/>
+      <c r="AIT1" s="41"/>
+      <c r="AIU1" s="41"/>
+      <c r="AIV1" s="41"/>
+      <c r="AIW1" s="41"/>
+      <c r="AIX1" s="41"/>
+      <c r="AIY1" s="41"/>
+      <c r="AIZ1" s="41"/>
+      <c r="AJA1" s="41"/>
+      <c r="AJB1" s="41"/>
+      <c r="AJC1" s="41"/>
+      <c r="AJD1" s="41"/>
+      <c r="AJE1" s="41"/>
+      <c r="AJF1" s="41"/>
+      <c r="AJG1" s="41"/>
+      <c r="AJH1" s="41"/>
+      <c r="AJI1" s="41"/>
+      <c r="AJJ1" s="41"/>
+      <c r="AJK1" s="41"/>
+      <c r="AJL1" s="41"/>
+      <c r="AJM1" s="41"/>
+      <c r="AJN1" s="41"/>
+      <c r="AJO1" s="41"/>
+      <c r="AJP1" s="41"/>
+      <c r="AJQ1" s="41"/>
+      <c r="AJR1" s="41"/>
+      <c r="AJS1" s="41"/>
+      <c r="AJT1" s="41"/>
+      <c r="AJU1" s="41"/>
+      <c r="AJV1" s="41"/>
+      <c r="AJW1" s="41"/>
+      <c r="AJX1" s="41"/>
+      <c r="AJY1" s="41"/>
+      <c r="AJZ1" s="41"/>
+      <c r="AKA1" s="41"/>
+      <c r="AKB1" s="41"/>
+      <c r="AKC1" s="41"/>
+      <c r="AKD1" s="41"/>
+      <c r="AKE1" s="41"/>
+      <c r="AKF1" s="41"/>
+      <c r="AKG1" s="41"/>
+      <c r="AKH1" s="41"/>
+      <c r="AKI1" s="41"/>
+      <c r="AKJ1" s="41"/>
+      <c r="AKK1" s="41"/>
+      <c r="AKL1" s="41"/>
+      <c r="AKM1" s="41"/>
+      <c r="AKN1" s="41"/>
+      <c r="AKO1" s="41"/>
+      <c r="AKP1" s="41"/>
+      <c r="AKQ1" s="41"/>
+      <c r="AKR1" s="41"/>
+      <c r="AKS1" s="41"/>
+      <c r="AKT1" s="41"/>
+      <c r="AKU1" s="41"/>
+      <c r="AKV1" s="41"/>
+      <c r="AKW1" s="41"/>
+      <c r="AKX1" s="41"/>
+      <c r="AKY1" s="41"/>
+      <c r="AKZ1" s="41"/>
+      <c r="ALA1" s="41"/>
+      <c r="ALB1" s="41"/>
+      <c r="ALC1" s="41"/>
+      <c r="ALD1" s="41"/>
+      <c r="ALE1" s="41"/>
+      <c r="ALF1" s="41"/>
+      <c r="ALG1" s="41"/>
+      <c r="ALH1" s="41"/>
+      <c r="ALI1" s="41"/>
+    </row>
+    <row r="2" spans="1:997" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>633</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>645</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>640</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>635</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="F2" s="29">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:997" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>634</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>646</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>643</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>635</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="F3" s="29">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:997" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>655</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>647</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>635</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="F4" s="29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:997" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>656</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>648</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>649</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>635</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>652</v>
+      </c>
+      <c r="F5" s="29">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:997" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>657</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>651</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>650</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>635</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>653</v>
+      </c>
+      <c r="F6" s="29">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALS6"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="58.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.140625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="41" customWidth="1"/>
+    <col min="4" max="4" width="52.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.85546875" style="29" customWidth="1"/>
+    <col min="6" max="6" width="11" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="1007" width="58.85546875" style="29"/>
+    <col min="1008" max="16384" width="58.85546875" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>81</v>
       </c>
       <c r="D1" s="18" t="s">
@@ -11901,99 +13162,108 @@
       <c r="ALM1" s="41"/>
       <c r="ALN1" s="41"/>
       <c r="ALO1" s="41"/>
-    </row>
-    <row r="2" spans="1:1003" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>633</v>
+      <c r="ALP1" s="41"/>
+      <c r="ALQ1" s="41"/>
+      <c r="ALR1" s="41"/>
+    </row>
+    <row r="2" spans="1:1006" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>636</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>645</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>640</v>
+        <v>660</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>658</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>641</v>
+        <v>671</v>
       </c>
       <c r="F2" s="29">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:1003" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>634</v>
+    <row r="3" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>637</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>646</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>643</v>
+        <v>661</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>659</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>642</v>
+        <v>672</v>
       </c>
       <c r="F3" s="29">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:1003" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+    <row r="4" spans="1:1006" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>638</v>
+      </c>
       <c r="B4" s="42" t="s">
-        <v>647</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>644</v>
+        <v>663</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>662</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>635</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>618</v>
+        <v>639</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>673</v>
       </c>
       <c r="F4" s="29">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1003" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1006" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>665</v>
+      </c>
       <c r="B5" s="42" t="s">
-        <v>648</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>596</v>
+        <v>667</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>664</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>629</v>
+        <v>670</v>
       </c>
       <c r="F5" s="29">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1003" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1006" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>668</v>
+      </c>
       <c r="B6" s="42" t="s">
-        <v>649</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>616</v>
+        <v>666</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>669</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="F6" s="29">
-        <v>200</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -12002,37 +13272,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM4"/>
+  <dimension ref="A1:AMM21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="58.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="105.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="70.42578125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="17" customWidth="1"/>
-    <col min="7" max="1027" width="58.85546875" style="17"/>
+    <col min="1" max="1" width="31.140625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="102.140625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="83" style="17" customWidth="1"/>
+    <col min="5" max="5" width="83.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="7" max="1025" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="40" t="s">
         <v>446</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>82</v>
@@ -12040,1085 +13310,309 @@
       <c r="F1" s="38" t="s">
         <v>576</v>
       </c>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-      <c r="AB1"/>
-      <c r="AC1"/>
-      <c r="AD1"/>
-      <c r="AE1"/>
-      <c r="AF1"/>
-      <c r="AG1"/>
-      <c r="AH1"/>
-      <c r="AI1"/>
-      <c r="AJ1"/>
-      <c r="AK1"/>
-      <c r="AL1"/>
-      <c r="AM1"/>
-      <c r="AN1"/>
-      <c r="AO1"/>
-      <c r="AP1"/>
-      <c r="AQ1"/>
-      <c r="AR1"/>
-      <c r="AS1"/>
-      <c r="AT1"/>
-      <c r="AU1"/>
-      <c r="AV1"/>
-      <c r="AW1"/>
-      <c r="AX1"/>
-      <c r="AY1"/>
-      <c r="AZ1"/>
-      <c r="BA1"/>
-      <c r="BB1"/>
-      <c r="BC1"/>
-      <c r="BD1"/>
-      <c r="BE1"/>
-      <c r="BF1"/>
-      <c r="BG1"/>
-      <c r="BH1"/>
-      <c r="BI1"/>
-      <c r="BJ1"/>
-      <c r="BK1"/>
-      <c r="BL1"/>
-      <c r="BM1"/>
-      <c r="BN1"/>
-      <c r="BO1"/>
-      <c r="BP1"/>
-      <c r="BQ1"/>
-      <c r="BR1"/>
-      <c r="BS1"/>
-      <c r="BT1"/>
-      <c r="BU1"/>
-      <c r="BV1"/>
-      <c r="BW1"/>
-      <c r="BX1"/>
-      <c r="BY1"/>
-      <c r="BZ1"/>
-      <c r="CA1"/>
-      <c r="CB1"/>
-      <c r="CC1"/>
-      <c r="CD1"/>
-      <c r="CE1"/>
-      <c r="CF1"/>
-      <c r="CG1"/>
-      <c r="CH1"/>
-      <c r="CI1"/>
-      <c r="CJ1"/>
-      <c r="CK1"/>
-      <c r="CL1"/>
-      <c r="CM1"/>
-      <c r="CN1"/>
-      <c r="CO1"/>
-      <c r="CP1"/>
-      <c r="CQ1"/>
-      <c r="CR1"/>
-      <c r="CS1"/>
-      <c r="CT1"/>
-      <c r="CU1"/>
-      <c r="CV1"/>
-      <c r="CW1"/>
-      <c r="CX1"/>
-      <c r="CY1"/>
-      <c r="CZ1"/>
-      <c r="DA1"/>
-      <c r="DB1"/>
-      <c r="DC1"/>
-      <c r="DD1"/>
-      <c r="DE1"/>
-      <c r="DF1"/>
-      <c r="DG1"/>
-      <c r="DH1"/>
-      <c r="DI1"/>
-      <c r="DJ1"/>
-      <c r="DK1"/>
-      <c r="DL1"/>
-      <c r="DM1"/>
-      <c r="DN1"/>
-      <c r="DO1"/>
-      <c r="DP1"/>
-      <c r="DQ1"/>
-      <c r="DR1"/>
-      <c r="DS1"/>
-      <c r="DT1"/>
-      <c r="DU1"/>
-      <c r="DV1"/>
-      <c r="DW1"/>
-      <c r="DX1"/>
-      <c r="DY1"/>
-      <c r="DZ1"/>
-      <c r="EA1"/>
-      <c r="EB1"/>
-      <c r="EC1"/>
-      <c r="ED1"/>
-      <c r="EE1"/>
-      <c r="EF1"/>
-      <c r="EG1"/>
-      <c r="EH1"/>
-      <c r="EI1"/>
-      <c r="EJ1"/>
-      <c r="EK1"/>
-      <c r="EL1"/>
-      <c r="EM1"/>
-      <c r="EN1"/>
-      <c r="EO1"/>
-      <c r="EP1"/>
-      <c r="EQ1"/>
-      <c r="ER1"/>
-      <c r="ES1"/>
-      <c r="ET1"/>
-      <c r="EU1"/>
-      <c r="EV1"/>
-      <c r="EW1"/>
-      <c r="EX1"/>
-      <c r="EY1"/>
-      <c r="EZ1"/>
-      <c r="FA1"/>
-      <c r="FB1"/>
-      <c r="FC1"/>
-      <c r="FD1"/>
-      <c r="FE1"/>
-      <c r="FF1"/>
-      <c r="FG1"/>
-      <c r="FH1"/>
-      <c r="FI1"/>
-      <c r="FJ1"/>
-      <c r="FK1"/>
-      <c r="FL1"/>
-      <c r="FM1"/>
-      <c r="FN1"/>
-      <c r="FO1"/>
-      <c r="FP1"/>
-      <c r="FQ1"/>
-      <c r="FR1"/>
-      <c r="FS1"/>
-      <c r="FT1"/>
-      <c r="FU1"/>
-      <c r="FV1"/>
-      <c r="FW1"/>
-      <c r="FX1"/>
-      <c r="FY1"/>
-      <c r="FZ1"/>
-      <c r="GA1"/>
-      <c r="GB1"/>
-      <c r="GC1"/>
-      <c r="GD1"/>
-      <c r="GE1"/>
-      <c r="GF1"/>
-      <c r="GG1"/>
-      <c r="GH1"/>
-      <c r="GI1"/>
-      <c r="GJ1"/>
-      <c r="GK1"/>
-      <c r="GL1"/>
-      <c r="GM1"/>
-      <c r="GN1"/>
-      <c r="GO1"/>
-      <c r="GP1"/>
-      <c r="GQ1"/>
-      <c r="GR1"/>
-      <c r="GS1"/>
-      <c r="GT1"/>
-      <c r="GU1"/>
-      <c r="GV1"/>
-      <c r="GW1"/>
-      <c r="GX1"/>
-      <c r="GY1"/>
-      <c r="GZ1"/>
-      <c r="HA1"/>
-      <c r="HB1"/>
-      <c r="HC1"/>
-      <c r="HD1"/>
-      <c r="HE1"/>
-      <c r="HF1"/>
-      <c r="HG1"/>
-      <c r="HH1"/>
-      <c r="HI1"/>
-      <c r="HJ1"/>
-      <c r="HK1"/>
-      <c r="HL1"/>
-      <c r="HM1"/>
-      <c r="HN1"/>
-      <c r="HO1"/>
-      <c r="HP1"/>
-      <c r="HQ1"/>
-      <c r="HR1"/>
-      <c r="HS1"/>
-      <c r="HT1"/>
-      <c r="HU1"/>
-      <c r="HV1"/>
-      <c r="HW1"/>
-      <c r="HX1"/>
-      <c r="HY1"/>
-      <c r="HZ1"/>
-      <c r="IA1"/>
-      <c r="IB1"/>
-      <c r="IC1"/>
-      <c r="ID1"/>
-      <c r="IE1"/>
-      <c r="IF1"/>
-      <c r="IG1"/>
-      <c r="IH1"/>
-      <c r="II1"/>
-      <c r="IJ1"/>
-      <c r="IK1"/>
-      <c r="IL1"/>
-      <c r="IM1"/>
-      <c r="IN1"/>
-      <c r="IO1"/>
-      <c r="IP1"/>
-      <c r="IQ1"/>
-      <c r="IR1"/>
-      <c r="IS1"/>
-      <c r="IT1"/>
-      <c r="IU1"/>
-      <c r="IV1"/>
-      <c r="IW1"/>
-      <c r="IX1"/>
-      <c r="IY1"/>
-      <c r="IZ1"/>
-      <c r="JA1"/>
-      <c r="JB1"/>
-      <c r="JC1"/>
-      <c r="JD1"/>
-      <c r="JE1"/>
-      <c r="JF1"/>
-      <c r="JG1"/>
-      <c r="JH1"/>
-      <c r="JI1"/>
-      <c r="JJ1"/>
-      <c r="JK1"/>
-      <c r="JL1"/>
-      <c r="JM1"/>
-      <c r="JN1"/>
-      <c r="JO1"/>
-      <c r="JP1"/>
-      <c r="JQ1"/>
-      <c r="JR1"/>
-      <c r="JS1"/>
-      <c r="JT1"/>
-      <c r="JU1"/>
-      <c r="JV1"/>
-      <c r="JW1"/>
-      <c r="JX1"/>
-      <c r="JY1"/>
-      <c r="JZ1"/>
-      <c r="KA1"/>
-      <c r="KB1"/>
-      <c r="KC1"/>
-      <c r="KD1"/>
-      <c r="KE1"/>
-      <c r="KF1"/>
-      <c r="KG1"/>
-      <c r="KH1"/>
-      <c r="KI1"/>
-      <c r="KJ1"/>
-      <c r="KK1"/>
-      <c r="KL1"/>
-      <c r="KM1"/>
-      <c r="KN1"/>
-      <c r="KO1"/>
-      <c r="KP1"/>
-      <c r="KQ1"/>
-      <c r="KR1"/>
-      <c r="KS1"/>
-      <c r="KT1"/>
-      <c r="KU1"/>
-      <c r="KV1"/>
-      <c r="KW1"/>
-      <c r="KX1"/>
-      <c r="KY1"/>
-      <c r="KZ1"/>
-      <c r="LA1"/>
-      <c r="LB1"/>
-      <c r="LC1"/>
-      <c r="LD1"/>
-      <c r="LE1"/>
-      <c r="LF1"/>
-      <c r="LG1"/>
-      <c r="LH1"/>
-      <c r="LI1"/>
-      <c r="LJ1"/>
-      <c r="LK1"/>
-      <c r="LL1"/>
-      <c r="LM1"/>
-      <c r="LN1"/>
-      <c r="LO1"/>
-      <c r="LP1"/>
-      <c r="LQ1"/>
-      <c r="LR1"/>
-      <c r="LS1"/>
-      <c r="LT1"/>
-      <c r="LU1"/>
-      <c r="LV1"/>
-      <c r="LW1"/>
-      <c r="LX1"/>
-      <c r="LY1"/>
-      <c r="LZ1"/>
-      <c r="MA1"/>
-      <c r="MB1"/>
-      <c r="MC1"/>
-      <c r="MD1"/>
-      <c r="ME1"/>
-      <c r="MF1"/>
-      <c r="MG1"/>
-      <c r="MH1"/>
-      <c r="MI1"/>
-      <c r="MJ1"/>
-      <c r="MK1"/>
-      <c r="ML1"/>
-      <c r="MM1"/>
-      <c r="MN1"/>
-      <c r="MO1"/>
-      <c r="MP1"/>
-      <c r="MQ1"/>
-      <c r="MR1"/>
-      <c r="MS1"/>
-      <c r="MT1"/>
-      <c r="MU1"/>
-      <c r="MV1"/>
-      <c r="MW1"/>
-      <c r="MX1"/>
-      <c r="MY1"/>
-      <c r="MZ1"/>
-      <c r="NA1"/>
-      <c r="NB1"/>
-      <c r="NC1"/>
-      <c r="ND1"/>
-      <c r="NE1"/>
-      <c r="NF1"/>
-      <c r="NG1"/>
-      <c r="NH1"/>
-      <c r="NI1"/>
-      <c r="NJ1"/>
-      <c r="NK1"/>
-      <c r="NL1"/>
-      <c r="NM1"/>
-      <c r="NN1"/>
-      <c r="NO1"/>
-      <c r="NP1"/>
-      <c r="NQ1"/>
-      <c r="NR1"/>
-      <c r="NS1"/>
-      <c r="NT1"/>
-      <c r="NU1"/>
-      <c r="NV1"/>
-      <c r="NW1"/>
-      <c r="NX1"/>
-      <c r="NY1"/>
-      <c r="NZ1"/>
-      <c r="OA1"/>
-      <c r="OB1"/>
-      <c r="OC1"/>
-      <c r="OD1"/>
-      <c r="OE1"/>
-      <c r="OF1"/>
-      <c r="OG1"/>
-      <c r="OH1"/>
-      <c r="OI1"/>
-      <c r="OJ1"/>
-      <c r="OK1"/>
-      <c r="OL1"/>
-      <c r="OM1"/>
-      <c r="ON1"/>
-      <c r="OO1"/>
-      <c r="OP1"/>
-      <c r="OQ1"/>
-      <c r="OR1"/>
-      <c r="OS1"/>
-      <c r="OT1"/>
-      <c r="OU1"/>
-      <c r="OV1"/>
-      <c r="OW1"/>
-      <c r="OX1"/>
-      <c r="OY1"/>
-      <c r="OZ1"/>
-      <c r="PA1"/>
-      <c r="PB1"/>
-      <c r="PC1"/>
-      <c r="PD1"/>
-      <c r="PE1"/>
-      <c r="PF1"/>
-      <c r="PG1"/>
-      <c r="PH1"/>
-      <c r="PI1"/>
-      <c r="PJ1"/>
-      <c r="PK1"/>
-      <c r="PL1"/>
-      <c r="PM1"/>
-      <c r="PN1"/>
-      <c r="PO1"/>
-      <c r="PP1"/>
-      <c r="PQ1"/>
-      <c r="PR1"/>
-      <c r="PS1"/>
-      <c r="PT1"/>
-      <c r="PU1"/>
-      <c r="PV1"/>
-      <c r="PW1"/>
-      <c r="PX1"/>
-      <c r="PY1"/>
-      <c r="PZ1"/>
-      <c r="QA1"/>
-      <c r="QB1"/>
-      <c r="QC1"/>
-      <c r="QD1"/>
-      <c r="QE1"/>
-      <c r="QF1"/>
-      <c r="QG1"/>
-      <c r="QH1"/>
-      <c r="QI1"/>
-      <c r="QJ1"/>
-      <c r="QK1"/>
-      <c r="QL1"/>
-      <c r="QM1"/>
-      <c r="QN1"/>
-      <c r="QO1"/>
-      <c r="QP1"/>
-      <c r="QQ1"/>
-      <c r="QR1"/>
-      <c r="QS1"/>
-      <c r="QT1"/>
-      <c r="QU1"/>
-      <c r="QV1"/>
-      <c r="QW1"/>
-      <c r="QX1"/>
-      <c r="QY1"/>
-      <c r="QZ1"/>
-      <c r="RA1"/>
-      <c r="RB1"/>
-      <c r="RC1"/>
-      <c r="RD1"/>
-      <c r="RE1"/>
-      <c r="RF1"/>
-      <c r="RG1"/>
-      <c r="RH1"/>
-      <c r="RI1"/>
-      <c r="RJ1"/>
-      <c r="RK1"/>
-      <c r="RL1"/>
-      <c r="RM1"/>
-      <c r="RN1"/>
-      <c r="RO1"/>
-      <c r="RP1"/>
-      <c r="RQ1"/>
-      <c r="RR1"/>
-      <c r="RS1"/>
-      <c r="RT1"/>
-      <c r="RU1"/>
-      <c r="RV1"/>
-      <c r="RW1"/>
-      <c r="RX1"/>
-      <c r="RY1"/>
-      <c r="RZ1"/>
-      <c r="SA1"/>
-      <c r="SB1"/>
-      <c r="SC1"/>
-      <c r="SD1"/>
-      <c r="SE1"/>
-      <c r="SF1"/>
-      <c r="SG1"/>
-      <c r="SH1"/>
-      <c r="SI1"/>
-      <c r="SJ1"/>
-      <c r="SK1"/>
-      <c r="SL1"/>
-      <c r="SM1"/>
-      <c r="SN1"/>
-      <c r="SO1"/>
-      <c r="SP1"/>
-      <c r="SQ1"/>
-      <c r="SR1"/>
-      <c r="SS1"/>
-      <c r="ST1"/>
-      <c r="SU1"/>
-      <c r="SV1"/>
-      <c r="SW1"/>
-      <c r="SX1"/>
-      <c r="SY1"/>
-      <c r="SZ1"/>
-      <c r="TA1"/>
-      <c r="TB1"/>
-      <c r="TC1"/>
-      <c r="TD1"/>
-      <c r="TE1"/>
-      <c r="TF1"/>
-      <c r="TG1"/>
-      <c r="TH1"/>
-      <c r="TI1"/>
-      <c r="TJ1"/>
-      <c r="TK1"/>
-      <c r="TL1"/>
-      <c r="TM1"/>
-      <c r="TN1"/>
-      <c r="TO1"/>
-      <c r="TP1"/>
-      <c r="TQ1"/>
-      <c r="TR1"/>
-      <c r="TS1"/>
-      <c r="TT1"/>
-      <c r="TU1"/>
-      <c r="TV1"/>
-      <c r="TW1"/>
-      <c r="TX1"/>
-      <c r="TY1"/>
-      <c r="TZ1"/>
-      <c r="UA1"/>
-      <c r="UB1"/>
-      <c r="UC1"/>
-      <c r="UD1"/>
-      <c r="UE1"/>
-      <c r="UF1"/>
-      <c r="UG1"/>
-      <c r="UH1"/>
-      <c r="UI1"/>
-      <c r="UJ1"/>
-      <c r="UK1"/>
-      <c r="UL1"/>
-      <c r="UM1"/>
-      <c r="UN1"/>
-      <c r="UO1"/>
-      <c r="UP1"/>
-      <c r="UQ1"/>
-      <c r="UR1"/>
-      <c r="US1"/>
-      <c r="UT1"/>
-      <c r="UU1"/>
-      <c r="UV1"/>
-      <c r="UW1"/>
-      <c r="UX1"/>
-      <c r="UY1"/>
-      <c r="UZ1"/>
-      <c r="VA1"/>
-      <c r="VB1"/>
-      <c r="VC1"/>
-      <c r="VD1"/>
-      <c r="VE1"/>
-      <c r="VF1"/>
-      <c r="VG1"/>
-      <c r="VH1"/>
-      <c r="VI1"/>
-      <c r="VJ1"/>
-      <c r="VK1"/>
-      <c r="VL1"/>
-      <c r="VM1"/>
-      <c r="VN1"/>
-      <c r="VO1"/>
-      <c r="VP1"/>
-      <c r="VQ1"/>
-      <c r="VR1"/>
-      <c r="VS1"/>
-      <c r="VT1"/>
-      <c r="VU1"/>
-      <c r="VV1"/>
-      <c r="VW1"/>
-      <c r="VX1"/>
-      <c r="VY1"/>
-      <c r="VZ1"/>
-      <c r="WA1"/>
-      <c r="WB1"/>
-      <c r="WC1"/>
-      <c r="WD1"/>
-      <c r="WE1"/>
-      <c r="WF1"/>
-      <c r="WG1"/>
-      <c r="WH1"/>
-      <c r="WI1"/>
-      <c r="WJ1"/>
-      <c r="WK1"/>
-      <c r="WL1"/>
-      <c r="WM1"/>
-      <c r="WN1"/>
-      <c r="WO1"/>
-      <c r="WP1"/>
-      <c r="WQ1"/>
-      <c r="WR1"/>
-      <c r="WS1"/>
-      <c r="WT1"/>
-      <c r="WU1"/>
-      <c r="WV1"/>
-      <c r="WW1"/>
-      <c r="WX1"/>
-      <c r="WY1"/>
-      <c r="WZ1"/>
-      <c r="XA1"/>
-      <c r="XB1"/>
-      <c r="XC1"/>
-      <c r="XD1"/>
-      <c r="XE1"/>
-      <c r="XF1"/>
-      <c r="XG1"/>
-      <c r="XH1"/>
-      <c r="XI1"/>
-      <c r="XJ1"/>
-      <c r="XK1"/>
-      <c r="XL1"/>
-      <c r="XM1"/>
-      <c r="XN1"/>
-      <c r="XO1"/>
-      <c r="XP1"/>
-      <c r="XQ1"/>
-      <c r="XR1"/>
-      <c r="XS1"/>
-      <c r="XT1"/>
-      <c r="XU1"/>
-      <c r="XV1"/>
-      <c r="XW1"/>
-      <c r="XX1"/>
-      <c r="XY1"/>
-      <c r="XZ1"/>
-      <c r="YA1"/>
-      <c r="YB1"/>
-      <c r="YC1"/>
-      <c r="YD1"/>
-      <c r="YE1"/>
-      <c r="YF1"/>
-      <c r="YG1"/>
-      <c r="YH1"/>
-      <c r="YI1"/>
-      <c r="YJ1"/>
-      <c r="YK1"/>
-      <c r="YL1"/>
-      <c r="YM1"/>
-      <c r="YN1"/>
-      <c r="YO1"/>
-      <c r="YP1"/>
-      <c r="YQ1"/>
-      <c r="YR1"/>
-      <c r="YS1"/>
-      <c r="YT1"/>
-      <c r="YU1"/>
-      <c r="YV1"/>
-      <c r="YW1"/>
-      <c r="YX1"/>
-      <c r="YY1"/>
-      <c r="YZ1"/>
-      <c r="ZA1"/>
-      <c r="ZB1"/>
-      <c r="ZC1"/>
-      <c r="ZD1"/>
-      <c r="ZE1"/>
-      <c r="ZF1"/>
-      <c r="ZG1"/>
-      <c r="ZH1"/>
-      <c r="ZI1"/>
-      <c r="ZJ1"/>
-      <c r="ZK1"/>
-      <c r="ZL1"/>
-      <c r="ZM1"/>
-      <c r="ZN1"/>
-      <c r="ZO1"/>
-      <c r="ZP1"/>
-      <c r="ZQ1"/>
-      <c r="ZR1"/>
-      <c r="ZS1"/>
-      <c r="ZT1"/>
-      <c r="ZU1"/>
-      <c r="ZV1"/>
-      <c r="ZW1"/>
-      <c r="ZX1"/>
-      <c r="ZY1"/>
-      <c r="ZZ1"/>
-      <c r="AAA1"/>
-      <c r="AAB1"/>
-      <c r="AAC1"/>
-      <c r="AAD1"/>
-      <c r="AAE1"/>
-      <c r="AAF1"/>
-      <c r="AAG1"/>
-      <c r="AAH1"/>
-      <c r="AAI1"/>
-      <c r="AAJ1"/>
-      <c r="AAK1"/>
-      <c r="AAL1"/>
-      <c r="AAM1"/>
-      <c r="AAN1"/>
-      <c r="AAO1"/>
-      <c r="AAP1"/>
-      <c r="AAQ1"/>
-      <c r="AAR1"/>
-      <c r="AAS1"/>
-      <c r="AAT1"/>
-      <c r="AAU1"/>
-      <c r="AAV1"/>
-      <c r="AAW1"/>
-      <c r="AAX1"/>
-      <c r="AAY1"/>
-      <c r="AAZ1"/>
-      <c r="ABA1"/>
-      <c r="ABB1"/>
-      <c r="ABC1"/>
-      <c r="ABD1"/>
-      <c r="ABE1"/>
-      <c r="ABF1"/>
-      <c r="ABG1"/>
-      <c r="ABH1"/>
-      <c r="ABI1"/>
-      <c r="ABJ1"/>
-      <c r="ABK1"/>
-      <c r="ABL1"/>
-      <c r="ABM1"/>
-      <c r="ABN1"/>
-      <c r="ABO1"/>
-      <c r="ABP1"/>
-      <c r="ABQ1"/>
-      <c r="ABR1"/>
-      <c r="ABS1"/>
-      <c r="ABT1"/>
-      <c r="ABU1"/>
-      <c r="ABV1"/>
-      <c r="ABW1"/>
-      <c r="ABX1"/>
-      <c r="ABY1"/>
-      <c r="ABZ1"/>
-      <c r="ACA1"/>
-      <c r="ACB1"/>
-      <c r="ACC1"/>
-      <c r="ACD1"/>
-      <c r="ACE1"/>
-      <c r="ACF1"/>
-      <c r="ACG1"/>
-      <c r="ACH1"/>
-      <c r="ACI1"/>
-      <c r="ACJ1"/>
-      <c r="ACK1"/>
-      <c r="ACL1"/>
-      <c r="ACM1"/>
-      <c r="ACN1"/>
-      <c r="ACO1"/>
-      <c r="ACP1"/>
-      <c r="ACQ1"/>
-      <c r="ACR1"/>
-      <c r="ACS1"/>
-      <c r="ACT1"/>
-      <c r="ACU1"/>
-      <c r="ACV1"/>
-      <c r="ACW1"/>
-      <c r="ACX1"/>
-      <c r="ACY1"/>
-      <c r="ACZ1"/>
-      <c r="ADA1"/>
-      <c r="ADB1"/>
-      <c r="ADC1"/>
-      <c r="ADD1"/>
-      <c r="ADE1"/>
-      <c r="ADF1"/>
-      <c r="ADG1"/>
-      <c r="ADH1"/>
-      <c r="ADI1"/>
-      <c r="ADJ1"/>
-      <c r="ADK1"/>
-      <c r="ADL1"/>
-      <c r="ADM1"/>
-      <c r="ADN1"/>
-      <c r="ADO1"/>
-      <c r="ADP1"/>
-      <c r="ADQ1"/>
-      <c r="ADR1"/>
-      <c r="ADS1"/>
-      <c r="ADT1"/>
-      <c r="ADU1"/>
-      <c r="ADV1"/>
-      <c r="ADW1"/>
-      <c r="ADX1"/>
-      <c r="ADY1"/>
-      <c r="ADZ1"/>
-      <c r="AEA1"/>
-      <c r="AEB1"/>
-      <c r="AEC1"/>
-      <c r="AED1"/>
-      <c r="AEE1"/>
-      <c r="AEF1"/>
-      <c r="AEG1"/>
-      <c r="AEH1"/>
-      <c r="AEI1"/>
-      <c r="AEJ1"/>
-      <c r="AEK1"/>
-      <c r="AEL1"/>
-      <c r="AEM1"/>
-      <c r="AEN1"/>
-      <c r="AEO1"/>
-      <c r="AEP1"/>
-      <c r="AEQ1"/>
-      <c r="AER1"/>
-      <c r="AES1"/>
-      <c r="AET1"/>
-      <c r="AEU1"/>
-      <c r="AEV1"/>
-      <c r="AEW1"/>
-      <c r="AEX1"/>
-      <c r="AEY1"/>
-      <c r="AEZ1"/>
-      <c r="AFA1"/>
-      <c r="AFB1"/>
-      <c r="AFC1"/>
-      <c r="AFD1"/>
-      <c r="AFE1"/>
-      <c r="AFF1"/>
-      <c r="AFG1"/>
-      <c r="AFH1"/>
-      <c r="AFI1"/>
-      <c r="AFJ1"/>
-      <c r="AFK1"/>
-      <c r="AFL1"/>
-      <c r="AFM1"/>
-      <c r="AFN1"/>
-      <c r="AFO1"/>
-      <c r="AFP1"/>
-      <c r="AFQ1"/>
-      <c r="AFR1"/>
-      <c r="AFS1"/>
-      <c r="AFT1"/>
-      <c r="AFU1"/>
-      <c r="AFV1"/>
-      <c r="AFW1"/>
-      <c r="AFX1"/>
-      <c r="AFY1"/>
-      <c r="AFZ1"/>
-      <c r="AGA1"/>
-      <c r="AGB1"/>
-      <c r="AGC1"/>
-      <c r="AGD1"/>
-      <c r="AGE1"/>
-      <c r="AGF1"/>
-      <c r="AGG1"/>
-      <c r="AGH1"/>
-      <c r="AGI1"/>
-      <c r="AGJ1"/>
-      <c r="AGK1"/>
-      <c r="AGL1"/>
-      <c r="AGM1"/>
-      <c r="AGN1"/>
-      <c r="AGO1"/>
-      <c r="AGP1"/>
-      <c r="AGQ1"/>
-      <c r="AGR1"/>
-      <c r="AGS1"/>
-      <c r="AGT1"/>
-      <c r="AGU1"/>
-      <c r="AGV1"/>
-      <c r="AGW1"/>
-      <c r="AGX1"/>
-      <c r="AGY1"/>
-      <c r="AGZ1"/>
-      <c r="AHA1"/>
-      <c r="AHB1"/>
-      <c r="AHC1"/>
-      <c r="AHD1"/>
-      <c r="AHE1"/>
-      <c r="AHF1"/>
-      <c r="AHG1"/>
-      <c r="AHH1"/>
-      <c r="AHI1"/>
-      <c r="AHJ1"/>
-      <c r="AHK1"/>
-      <c r="AHL1"/>
-      <c r="AHM1"/>
-      <c r="AHN1"/>
-      <c r="AHO1"/>
-      <c r="AHP1"/>
-      <c r="AHQ1"/>
-      <c r="AHR1"/>
-      <c r="AHS1"/>
-      <c r="AHT1"/>
-      <c r="AHU1"/>
-      <c r="AHV1"/>
-      <c r="AHW1"/>
-      <c r="AHX1"/>
-      <c r="AHY1"/>
-      <c r="AHZ1"/>
-      <c r="AIA1"/>
-      <c r="AIB1"/>
-      <c r="AIC1"/>
-      <c r="AID1"/>
-      <c r="AIE1"/>
-      <c r="AIF1"/>
-      <c r="AIG1"/>
-      <c r="AIH1"/>
-      <c r="AII1"/>
-      <c r="AIJ1"/>
-      <c r="AIK1"/>
-      <c r="AIL1"/>
-      <c r="AIM1"/>
-      <c r="AIN1"/>
-      <c r="AIO1"/>
-      <c r="AIP1"/>
-      <c r="AIQ1"/>
-      <c r="AIR1"/>
-      <c r="AIS1"/>
-      <c r="AIT1"/>
-      <c r="AIU1"/>
-      <c r="AIV1"/>
-      <c r="AIW1"/>
-      <c r="AIX1"/>
-      <c r="AIY1"/>
-      <c r="AIZ1"/>
-      <c r="AJA1"/>
-      <c r="AJB1"/>
-      <c r="AJC1"/>
-      <c r="AJD1"/>
-      <c r="AJE1"/>
-      <c r="AJF1"/>
-      <c r="AJG1"/>
-      <c r="AJH1"/>
-      <c r="AJI1"/>
-      <c r="AJJ1"/>
-      <c r="AJK1"/>
-      <c r="AJL1"/>
-      <c r="AJM1"/>
-      <c r="AJN1"/>
-      <c r="AJO1"/>
-      <c r="AJP1"/>
-      <c r="AJQ1"/>
-      <c r="AJR1"/>
-      <c r="AJS1"/>
-      <c r="AJT1"/>
-      <c r="AJU1"/>
-      <c r="AJV1"/>
-      <c r="AJW1"/>
-      <c r="AJX1"/>
-      <c r="AJY1"/>
-      <c r="AJZ1"/>
-      <c r="AKA1"/>
-      <c r="AKB1"/>
-      <c r="AKC1"/>
-      <c r="AKD1"/>
-      <c r="AKE1"/>
-      <c r="AKF1"/>
-      <c r="AKG1"/>
-      <c r="AKH1"/>
-      <c r="AKI1"/>
-      <c r="AKJ1"/>
-      <c r="AKK1"/>
-      <c r="AKL1"/>
-      <c r="AKM1"/>
-      <c r="AKN1"/>
-      <c r="AKO1"/>
-      <c r="AKP1"/>
-      <c r="AKQ1"/>
-      <c r="AKR1"/>
-      <c r="AKS1"/>
-      <c r="AKT1"/>
-      <c r="AKU1"/>
-      <c r="AKV1"/>
-      <c r="AKW1"/>
-      <c r="AKX1"/>
-      <c r="AKY1"/>
-      <c r="AKZ1"/>
-      <c r="ALA1"/>
-      <c r="ALB1"/>
-      <c r="ALC1"/>
-      <c r="ALD1"/>
-      <c r="ALE1"/>
-      <c r="ALF1"/>
-      <c r="ALG1"/>
-      <c r="ALH1"/>
-      <c r="ALI1"/>
-      <c r="ALJ1"/>
-      <c r="ALK1"/>
-      <c r="ALL1"/>
-      <c r="ALM1"/>
-      <c r="ALN1"/>
-      <c r="ALO1"/>
-      <c r="ALP1"/>
-      <c r="ALQ1"/>
-      <c r="ALR1"/>
-      <c r="ALS1"/>
-      <c r="ALT1"/>
-      <c r="ALU1"/>
-      <c r="ALV1"/>
-      <c r="ALW1"/>
-      <c r="ALX1"/>
-      <c r="ALY1"/>
-      <c r="ALZ1"/>
-      <c r="AMA1"/>
-      <c r="AMB1"/>
-      <c r="AMC1"/>
-      <c r="AMD1"/>
-      <c r="AME1"/>
-      <c r="AMF1"/>
-      <c r="AMG1"/>
-      <c r="AMH1"/>
-      <c r="AMI1"/>
-      <c r="AMJ1"/>
-      <c r="AMK1"/>
-      <c r="AML1"/>
-    </row>
-    <row r="2" spans="1:1026" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>603</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>607</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>639</v>
+      <c r="AML1" s="17"/>
+      <c r="AMM1" s="17"/>
+    </row>
+    <row r="2" spans="1:6 1026:1027" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>674</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>682</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>687</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="F2" s="17">
+        <v>219</v>
+      </c>
+      <c r="F2" s="43">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>637</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>604</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>602</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>639</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>620</v>
-      </c>
-      <c r="F3" s="17">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>638</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>615</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="AML2" s="17"/>
+      <c r="AMM2" s="17"/>
+    </row>
+    <row r="3" spans="1:6 1026:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>675</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>684</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>688</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="43"/>
+      <c r="AML3" s="17"/>
+      <c r="AMM3" s="17"/>
+    </row>
+    <row r="4" spans="1:6 1026:1027" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>676</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>683</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>689</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="43"/>
+      <c r="AML4" s="17"/>
+      <c r="AMM4" s="17"/>
+    </row>
+    <row r="5" spans="1:6 1026:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>677</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>685</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>690</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="43"/>
+      <c r="AML5" s="17"/>
+      <c r="AMM5" s="17"/>
+    </row>
+    <row r="6" spans="1:6 1026:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="42" t="s">
+        <v>686</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="43"/>
+      <c r="AML6" s="17"/>
+      <c r="AMM6" s="17"/>
+    </row>
+    <row r="7" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="43"/>
+      <c r="AML7" s="17"/>
+      <c r="AMM7" s="17"/>
+    </row>
+    <row r="8" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="43"/>
+      <c r="AML8" s="17"/>
+      <c r="AMM8" s="17"/>
+    </row>
+    <row r="9" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="43"/>
+      <c r="AML9" s="17"/>
+      <c r="AMM9" s="17"/>
+    </row>
+    <row r="10" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="43"/>
+      <c r="AML10" s="17"/>
+      <c r="AMM10" s="17"/>
+    </row>
+    <row r="11" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="43"/>
+      <c r="AML11" s="17"/>
+      <c r="AMM11" s="17"/>
+    </row>
+    <row r="12" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="43"/>
+      <c r="AML12" s="17"/>
+      <c r="AMM12" s="17"/>
+    </row>
+    <row r="13" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="43"/>
+      <c r="AML13" s="17"/>
+      <c r="AMM13" s="17"/>
+    </row>
+    <row r="14" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="43"/>
+      <c r="AML14" s="17"/>
+      <c r="AMM14" s="17"/>
+    </row>
+    <row r="15" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="43"/>
+      <c r="AML15" s="17"/>
+      <c r="AMM15" s="17"/>
+    </row>
+    <row r="16" spans="1:6 1026:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>675</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>578</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="F16" s="43">
+        <v>200</v>
+      </c>
+      <c r="AML16" s="17"/>
+      <c r="AMM16" s="17"/>
+    </row>
+    <row r="17" spans="1:6 1026:1027" ht="225" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>676</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>579</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F17" s="43">
+        <v>400</v>
+      </c>
+      <c r="AML17" s="17"/>
+      <c r="AMM17" s="17"/>
+    </row>
+    <row r="18" spans="1:6 1026:1027" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>677</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>580</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="F18" s="43">
+        <v>400</v>
+      </c>
+      <c r="AML18" s="17"/>
+      <c r="AMM18" s="17"/>
+    </row>
+    <row r="19" spans="1:6 1026:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>678</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>581</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F19" s="43">
+        <v>409</v>
+      </c>
+      <c r="AML19" s="17"/>
+      <c r="AMM19" s="17"/>
+    </row>
+    <row r="20" spans="1:6 1026:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>679</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>582</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="F20" s="43">
+        <v>400</v>
+      </c>
+      <c r="AML20" s="17"/>
+      <c r="AMM20" s="17"/>
+    </row>
+    <row r="21" spans="1:6 1026:1027" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>680</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>639</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>621</v>
-      </c>
-      <c r="F4" s="17">
-        <v>400</v>
+      <c r="E21" s="22" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>